<commit_message>
add kanji lesson 2
</commit_message>
<xml_diff>
--- a/Review_Kanji_V2/Lesson2/kanjiv2.xlsx
+++ b/Review_Kanji_V2/Lesson2/kanjiv2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\01_LearningJapaneseWebProject\Review_Kanji_V2\Lesson2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FE31CFA-486E-487C-A174-377E6E588195}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CE6FA15-4FFF-49B9-98A0-40E59C5A8525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1665" yWindow="1290" windowWidth="21495" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9240" yWindow="1815" windowWidth="21495" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="552">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1088" uniqueCount="1028">
   <si>
     <t>japanese</t>
   </si>
@@ -1681,6 +1681,1434 @@
   </si>
   <si>
     <t>第二課</t>
+  </si>
+  <si>
+    <t>枚</t>
+  </si>
+  <si>
+    <t>mai</t>
+  </si>
+  <si>
+    <t>杯</t>
+  </si>
+  <si>
+    <t>bôi</t>
+  </si>
+  <si>
+    <t>đếm ly, chén</t>
+  </si>
+  <si>
+    <t>柔</t>
+  </si>
+  <si>
+    <t>nhu</t>
+  </si>
+  <si>
+    <t>mềm</t>
+  </si>
+  <si>
+    <t>案</t>
+  </si>
+  <si>
+    <t>án</t>
+  </si>
+  <si>
+    <t>hướng dẫn</t>
+  </si>
+  <si>
+    <t>格</t>
+  </si>
+  <si>
+    <t>cách</t>
+  </si>
+  <si>
+    <t>tư cách</t>
+  </si>
+  <si>
+    <t>械</t>
+  </si>
+  <si>
+    <t>cơ giới</t>
+  </si>
+  <si>
+    <t>植</t>
+  </si>
+  <si>
+    <t>thực</t>
+  </si>
+  <si>
+    <t>thực vật</t>
+  </si>
+  <si>
+    <t>棒</t>
+  </si>
+  <si>
+    <t>棚</t>
+  </si>
+  <si>
+    <t>様</t>
+  </si>
+  <si>
+    <t>bổng</t>
+  </si>
+  <si>
+    <t>cây gậy</t>
+  </si>
+  <si>
+    <t>bằng</t>
+  </si>
+  <si>
+    <t>cái kệ</t>
+  </si>
+  <si>
+    <t>dạng</t>
+  </si>
+  <si>
+    <t>hình dạng</t>
+  </si>
+  <si>
+    <t>橫</t>
+  </si>
+  <si>
+    <t>hoành</t>
+  </si>
+  <si>
+    <t>chiều ngang</t>
+  </si>
+  <si>
+    <t>機</t>
+  </si>
+  <si>
+    <t>cơ</t>
+  </si>
+  <si>
+    <t>橋</t>
+  </si>
+  <si>
+    <t>kiều</t>
+  </si>
+  <si>
+    <t>cầu</t>
+  </si>
+  <si>
+    <t>次</t>
+  </si>
+  <si>
+    <t>thứ</t>
+  </si>
+  <si>
+    <t>kế tiếp</t>
+  </si>
+  <si>
+    <t>歳</t>
+  </si>
+  <si>
+    <t>tuế</t>
+  </si>
+  <si>
+    <t>tuổi, năm</t>
+  </si>
+  <si>
+    <t>残</t>
+  </si>
+  <si>
+    <t>tàn</t>
+  </si>
+  <si>
+    <t>tàn dư</t>
+  </si>
+  <si>
+    <t>段</t>
+  </si>
+  <si>
+    <t>比</t>
+  </si>
+  <si>
+    <t>đoạn</t>
+  </si>
+  <si>
+    <t>giai đoạn</t>
+  </si>
+  <si>
+    <t>tỷ</t>
+  </si>
+  <si>
+    <t>so sánh</t>
+  </si>
+  <si>
+    <t>氷</t>
+  </si>
+  <si>
+    <t>汚</t>
+  </si>
+  <si>
+    <t>băng</t>
+  </si>
+  <si>
+    <t>tảng băng</t>
+  </si>
+  <si>
+    <t>ô</t>
+  </si>
+  <si>
+    <t>ô nhiễm</t>
+  </si>
+  <si>
+    <t>汗</t>
+  </si>
+  <si>
+    <t>決</t>
+  </si>
+  <si>
+    <t>治</t>
+  </si>
+  <si>
+    <t>泉</t>
+  </si>
+  <si>
+    <t>波</t>
+  </si>
+  <si>
+    <t>油</t>
+  </si>
+  <si>
+    <t>泥</t>
+  </si>
+  <si>
+    <t>hãn</t>
+  </si>
+  <si>
+    <t>mồ hôi</t>
+  </si>
+  <si>
+    <t>quyết</t>
+  </si>
+  <si>
+    <t>quyết định</t>
+  </si>
+  <si>
+    <t>chữa trị</t>
+  </si>
+  <si>
+    <t>tuyền</t>
+  </si>
+  <si>
+    <t>suối</t>
+  </si>
+  <si>
+    <t>ba</t>
+  </si>
+  <si>
+    <t>con sóng</t>
+  </si>
+  <si>
+    <t>du</t>
+  </si>
+  <si>
+    <t>dầu</t>
+  </si>
+  <si>
+    <t>nê</t>
+  </si>
+  <si>
+    <t>bùn</t>
+  </si>
+  <si>
+    <t>泊</t>
+  </si>
+  <si>
+    <t>沸</t>
+  </si>
+  <si>
+    <t>洋</t>
+  </si>
+  <si>
+    <t>trọ lại</t>
+  </si>
+  <si>
+    <t>phí</t>
+  </si>
+  <si>
+    <t>đun sôi</t>
+  </si>
+  <si>
+    <t>đại dương</t>
+  </si>
+  <si>
+    <t>流</t>
+  </si>
+  <si>
+    <t>淚</t>
+  </si>
+  <si>
+    <t>減</t>
+  </si>
+  <si>
+    <t>湖</t>
+  </si>
+  <si>
+    <t>湯</t>
+  </si>
+  <si>
+    <t>渡</t>
+  </si>
+  <si>
+    <t>源</t>
+  </si>
+  <si>
+    <t>lưu</t>
+  </si>
+  <si>
+    <t>chảy</t>
+  </si>
+  <si>
+    <t>nước mắt</t>
+  </si>
+  <si>
+    <t>giảm</t>
+  </si>
+  <si>
+    <t>hồ</t>
+  </si>
+  <si>
+    <t>cái hồ</t>
+  </si>
+  <si>
+    <t>thang</t>
+  </si>
+  <si>
+    <t>nước sôi</t>
+  </si>
+  <si>
+    <t>độ</t>
+  </si>
+  <si>
+    <t>băng qua</t>
+  </si>
+  <si>
+    <t>nguồn</t>
+  </si>
+  <si>
+    <t>準</t>
+  </si>
+  <si>
+    <t>濃</t>
+  </si>
+  <si>
+    <t>濯</t>
+  </si>
+  <si>
+    <t>chuẩn</t>
+  </si>
+  <si>
+    <t>nồng</t>
+  </si>
+  <si>
+    <t>đậm đặc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">trạc </t>
+  </si>
+  <si>
+    <t>rửa, giặt</t>
+  </si>
+  <si>
+    <t>đếm vật mỏng, tờ</t>
+  </si>
+  <si>
+    <t>灰</t>
+  </si>
+  <si>
+    <t>燒</t>
+  </si>
+  <si>
+    <t>然</t>
+  </si>
+  <si>
+    <t>無</t>
+  </si>
+  <si>
+    <t>煙</t>
+  </si>
+  <si>
+    <t>hôi</t>
+  </si>
+  <si>
+    <t>tro</t>
+  </si>
+  <si>
+    <t>thiêu</t>
+  </si>
+  <si>
+    <t>nướng</t>
+  </si>
+  <si>
+    <t>nhiên</t>
+  </si>
+  <si>
+    <t>tự nhiên</t>
+  </si>
+  <si>
+    <t>vô</t>
+  </si>
+  <si>
+    <t>vô lý</t>
+  </si>
+  <si>
+    <t>yên</t>
+  </si>
+  <si>
+    <t>khói</t>
+  </si>
+  <si>
+    <t>熱</t>
+  </si>
+  <si>
+    <t>燃</t>
+  </si>
+  <si>
+    <t>片</t>
+  </si>
+  <si>
+    <t>特</t>
+  </si>
+  <si>
+    <t>独</t>
+  </si>
+  <si>
+    <t>nhiệt</t>
+  </si>
+  <si>
+    <t>nóng</t>
+  </si>
+  <si>
+    <t>nhiên liệu</t>
+  </si>
+  <si>
+    <t>phiến</t>
+  </si>
+  <si>
+    <t>một chiều</t>
+  </si>
+  <si>
+    <t>đặc</t>
+  </si>
+  <si>
+    <t>đặt biệt</t>
+  </si>
+  <si>
+    <t>độc</t>
+  </si>
+  <si>
+    <t>độc thân</t>
+  </si>
+  <si>
+    <t>的</t>
+  </si>
+  <si>
+    <t>直</t>
+  </si>
+  <si>
+    <t>県</t>
+  </si>
+  <si>
+    <t>相</t>
+  </si>
+  <si>
+    <t>眠</t>
+  </si>
+  <si>
+    <t>眼</t>
+  </si>
+  <si>
+    <t>破</t>
+  </si>
+  <si>
+    <t>đích</t>
+  </si>
+  <si>
+    <t>mục đích</t>
+  </si>
+  <si>
+    <t>trực</t>
+  </si>
+  <si>
+    <t>sửa chữa</t>
+  </si>
+  <si>
+    <t>huyện</t>
+  </si>
+  <si>
+    <t>tỉnh</t>
+  </si>
+  <si>
+    <t>tương</t>
+  </si>
+  <si>
+    <t>tương lỗ</t>
+  </si>
+  <si>
+    <t>miên</t>
+  </si>
+  <si>
+    <t>buồn ngủ</t>
+  </si>
+  <si>
+    <t>con mắt</t>
+  </si>
+  <si>
+    <t>phá</t>
+  </si>
+  <si>
+    <t>rách</t>
+  </si>
+  <si>
+    <t>確</t>
+  </si>
+  <si>
+    <t>示</t>
+  </si>
+  <si>
+    <t>祈</t>
+  </si>
+  <si>
+    <t>xác</t>
+  </si>
+  <si>
+    <t>xác nhận</t>
+  </si>
+  <si>
+    <t>thị</t>
+  </si>
+  <si>
+    <t>chỉ thị</t>
+  </si>
+  <si>
+    <t>cầu xin</t>
+  </si>
+  <si>
+    <t>神</t>
+  </si>
+  <si>
+    <t>祖</t>
+  </si>
+  <si>
+    <t>禁</t>
+  </si>
+  <si>
+    <t>科</t>
+  </si>
+  <si>
+    <t>種</t>
+  </si>
+  <si>
+    <t>thần</t>
+  </si>
+  <si>
+    <t>thần thánh</t>
+  </si>
+  <si>
+    <t>tổ</t>
+  </si>
+  <si>
+    <t>tổ phụ, tôt</t>
+  </si>
+  <si>
+    <t>cấm</t>
+  </si>
+  <si>
+    <t>ngăn cấm</t>
+  </si>
+  <si>
+    <t>khoa</t>
+  </si>
+  <si>
+    <t>khoa học</t>
+  </si>
+  <si>
+    <t>税</t>
+  </si>
+  <si>
+    <t>thuế</t>
+  </si>
+  <si>
+    <t>tiền thuế</t>
+  </si>
+  <si>
+    <t>chủng</t>
+  </si>
+  <si>
+    <t>chủng loại</t>
+  </si>
+  <si>
+    <t>第</t>
+  </si>
+  <si>
+    <t>符</t>
+  </si>
+  <si>
+    <t>筆</t>
+  </si>
+  <si>
+    <t>節</t>
+  </si>
+  <si>
+    <t>管</t>
+  </si>
+  <si>
+    <t>算</t>
+  </si>
+  <si>
+    <t>築</t>
+  </si>
+  <si>
+    <t>đệ</t>
+  </si>
+  <si>
+    <t>thứ tự</t>
+  </si>
+  <si>
+    <t>phù</t>
+  </si>
+  <si>
+    <t>phù hiệu</t>
+  </si>
+  <si>
+    <t>bút</t>
+  </si>
+  <si>
+    <t>bút lông</t>
+  </si>
+  <si>
+    <t>tiết</t>
+  </si>
+  <si>
+    <t>thời tiết</t>
+  </si>
+  <si>
+    <t>quản</t>
+  </si>
+  <si>
+    <t>quản lý</t>
+  </si>
+  <si>
+    <t>toán</t>
+  </si>
+  <si>
+    <t>tính toán</t>
+  </si>
+  <si>
+    <t>trúc</t>
+  </si>
+  <si>
+    <t>kiến trúc, xây cất</t>
+  </si>
+  <si>
+    <t>細</t>
+  </si>
+  <si>
+    <t>組</t>
+  </si>
+  <si>
+    <t>給</t>
+  </si>
+  <si>
+    <t>絶</t>
+  </si>
+  <si>
+    <t>絡</t>
+  </si>
+  <si>
+    <t>続</t>
+  </si>
+  <si>
+    <t>簡</t>
+  </si>
+  <si>
+    <t>紀</t>
+  </si>
+  <si>
+    <t>級</t>
+  </si>
+  <si>
+    <t>giản</t>
+  </si>
+  <si>
+    <t>kỷ</t>
+  </si>
+  <si>
+    <t>thế kỷ</t>
+  </si>
+  <si>
+    <t>cấp</t>
+  </si>
+  <si>
+    <t>cấp độ</t>
+  </si>
+  <si>
+    <t>thon, chi tiết</t>
+  </si>
+  <si>
+    <t>tổ chức</t>
+  </si>
+  <si>
+    <t>tuyệt</t>
+  </si>
+  <si>
+    <t>tuyệt đối</t>
+  </si>
+  <si>
+    <t>tục</t>
+  </si>
+  <si>
+    <t>tiếp tục</t>
+  </si>
+  <si>
+    <t>緑</t>
+  </si>
+  <si>
+    <t>線</t>
+  </si>
+  <si>
+    <t>缶</t>
+  </si>
+  <si>
+    <t>lục</t>
+  </si>
+  <si>
+    <t>xanh lá cây</t>
+  </si>
+  <si>
+    <t>tuyến</t>
+  </si>
+  <si>
+    <t>tuyến đường</t>
+  </si>
+  <si>
+    <t>phẫu</t>
+  </si>
+  <si>
+    <t>cái lon</t>
+  </si>
+  <si>
+    <t>究</t>
+  </si>
+  <si>
+    <t>窓</t>
+  </si>
+  <si>
+    <t>置</t>
+  </si>
+  <si>
+    <t>竹</t>
+  </si>
+  <si>
+    <t>nghiên cứu</t>
+  </si>
+  <si>
+    <t>song</t>
+  </si>
+  <si>
+    <t>cửa sổ</t>
+  </si>
+  <si>
+    <t>trí</t>
+  </si>
+  <si>
+    <t>bố trí</t>
+  </si>
+  <si>
+    <t>tre, trúc</t>
+  </si>
+  <si>
+    <t>絵</t>
+  </si>
+  <si>
+    <t>hội</t>
+  </si>
+  <si>
+    <t>hội hoạ</t>
+  </si>
+  <si>
+    <t>美</t>
+  </si>
+  <si>
+    <t>義</t>
+  </si>
+  <si>
+    <t>育</t>
+  </si>
+  <si>
+    <t>胃</t>
+  </si>
+  <si>
+    <t>背</t>
+  </si>
+  <si>
+    <t>能</t>
+  </si>
+  <si>
+    <t>船</t>
+  </si>
+  <si>
+    <t>術</t>
+  </si>
+  <si>
+    <t>衣</t>
+  </si>
+  <si>
+    <t>mĩ</t>
+  </si>
+  <si>
+    <t>đẹp</t>
+  </si>
+  <si>
+    <t>nghĩa</t>
+  </si>
+  <si>
+    <t>nghĩa vụ</t>
+  </si>
+  <si>
+    <t>dục</t>
+  </si>
+  <si>
+    <t>dạ dày</t>
+  </si>
+  <si>
+    <t>bối</t>
+  </si>
+  <si>
+    <t>cái lưng</t>
+  </si>
+  <si>
+    <t>năng</t>
+  </si>
+  <si>
+    <t>năng  lực</t>
+  </si>
+  <si>
+    <t>thuyền</t>
+  </si>
+  <si>
+    <t>tàu, thuyền</t>
+  </si>
+  <si>
+    <t>thuật</t>
+  </si>
+  <si>
+    <t xml:space="preserve">y </t>
+  </si>
+  <si>
+    <t>y phục</t>
+  </si>
+  <si>
+    <t>giáo dục</t>
+  </si>
+  <si>
+    <t>脱</t>
+  </si>
+  <si>
+    <t>thoát</t>
+  </si>
+  <si>
+    <t>cơi, thoát y</t>
+  </si>
+  <si>
+    <t>表</t>
+  </si>
+  <si>
+    <t>袋</t>
+  </si>
+  <si>
+    <t>裏</t>
+  </si>
+  <si>
+    <t>製</t>
+  </si>
+  <si>
+    <t>複</t>
+  </si>
+  <si>
+    <t>規</t>
+  </si>
+  <si>
+    <t>覚</t>
+  </si>
+  <si>
+    <t>覧</t>
+  </si>
+  <si>
+    <t>解</t>
+  </si>
+  <si>
+    <t>角</t>
+  </si>
+  <si>
+    <t>biểu</t>
+  </si>
+  <si>
+    <t>biểu hiện</t>
+  </si>
+  <si>
+    <t>bap, túi</t>
+  </si>
+  <si>
+    <t>lí</t>
+  </si>
+  <si>
+    <t>mặt sau</t>
+  </si>
+  <si>
+    <t>chế</t>
+  </si>
+  <si>
+    <t>chế tao, tạo ra</t>
+  </si>
+  <si>
+    <t>phức</t>
+  </si>
+  <si>
+    <t>phức tạp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">quy </t>
+  </si>
+  <si>
+    <t>giác</t>
+  </si>
+  <si>
+    <t>nhớ</t>
+  </si>
+  <si>
+    <t>lãm</t>
+  </si>
+  <si>
+    <t>triễn lãm</t>
+  </si>
+  <si>
+    <t>giải</t>
+  </si>
+  <si>
+    <t>giải quyết</t>
+  </si>
+  <si>
+    <t>góc độ</t>
+  </si>
+  <si>
+    <t>触</t>
+  </si>
+  <si>
+    <t>許</t>
+  </si>
+  <si>
+    <t>訳</t>
+  </si>
+  <si>
+    <t>詰</t>
+  </si>
+  <si>
+    <t>xúc</t>
+  </si>
+  <si>
+    <t>tiếp xúc</t>
+  </si>
+  <si>
+    <t>hứa</t>
+  </si>
+  <si>
+    <t>cho phép</t>
+  </si>
+  <si>
+    <t>phiên dịch</t>
+  </si>
+  <si>
+    <t>cật</t>
+  </si>
+  <si>
+    <t>dồn, nhét</t>
+  </si>
+  <si>
+    <t>詳</t>
+  </si>
+  <si>
+    <t>認</t>
+  </si>
+  <si>
+    <t>誘</t>
+  </si>
+  <si>
+    <t>課</t>
+  </si>
+  <si>
+    <t>談</t>
+  </si>
+  <si>
+    <t>調</t>
+  </si>
+  <si>
+    <t>tường</t>
+  </si>
+  <si>
+    <t>chi tiết</t>
+  </si>
+  <si>
+    <t>nhận</t>
+  </si>
+  <si>
+    <t>công nhận</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dụ </t>
+  </si>
+  <si>
+    <t>rủ rê</t>
+  </si>
+  <si>
+    <t>khoá</t>
+  </si>
+  <si>
+    <t>bài học</t>
+  </si>
+  <si>
+    <t>đàm</t>
+  </si>
+  <si>
+    <t>đàm thoại</t>
+  </si>
+  <si>
+    <t>điều</t>
+  </si>
+  <si>
+    <t>điều tra</t>
+  </si>
+  <si>
+    <t>論</t>
+  </si>
+  <si>
+    <t>講</t>
+  </si>
+  <si>
+    <t>謝</t>
+  </si>
+  <si>
+    <t>警</t>
+  </si>
+  <si>
+    <t>議</t>
+  </si>
+  <si>
+    <t>象</t>
+  </si>
+  <si>
+    <t>負</t>
+  </si>
+  <si>
+    <t>貯</t>
+  </si>
+  <si>
+    <t>費</t>
+  </si>
+  <si>
+    <t>貿</t>
+  </si>
+  <si>
+    <t>luận</t>
+  </si>
+  <si>
+    <t>luận văn</t>
+  </si>
+  <si>
+    <t>giảng</t>
+  </si>
+  <si>
+    <t>giảng giải</t>
+  </si>
+  <si>
+    <t>tạ</t>
+  </si>
+  <si>
+    <t>khuyến cáo</t>
+  </si>
+  <si>
+    <t>nghị</t>
+  </si>
+  <si>
+    <t>hội nghị</t>
+  </si>
+  <si>
+    <t>tượng</t>
+  </si>
+  <si>
+    <t>cá voi</t>
+  </si>
+  <si>
+    <t>phụ</t>
+  </si>
+  <si>
+    <t>thua</t>
+  </si>
+  <si>
+    <t>trữ</t>
+  </si>
+  <si>
+    <t>tích trữ</t>
+  </si>
+  <si>
+    <t>chi phí</t>
+  </si>
+  <si>
+    <t>mậu</t>
+  </si>
+  <si>
+    <t>mậu dịch</t>
+  </si>
+  <si>
+    <t>tạ lỗi, tạ ơn</t>
+  </si>
+  <si>
+    <t>資</t>
+  </si>
+  <si>
+    <t>賃</t>
+  </si>
+  <si>
+    <t>賛</t>
+  </si>
+  <si>
+    <t>質</t>
+  </si>
+  <si>
+    <t>農</t>
+  </si>
+  <si>
+    <t>醉</t>
+  </si>
+  <si>
+    <t>野</t>
+  </si>
+  <si>
+    <t>量</t>
+  </si>
+  <si>
+    <t>賞</t>
+  </si>
+  <si>
+    <t>贈</t>
+  </si>
+  <si>
+    <t>越</t>
+  </si>
+  <si>
+    <t>趣</t>
+  </si>
+  <si>
+    <t>舞</t>
+  </si>
+  <si>
+    <t>踊</t>
+  </si>
+  <si>
+    <t>踏</t>
+  </si>
+  <si>
+    <t>身</t>
+  </si>
+  <si>
+    <t>輸</t>
+  </si>
+  <si>
+    <t>麦</t>
+  </si>
+  <si>
+    <t>鉄</t>
+  </si>
+  <si>
+    <t>鉛</t>
+  </si>
+  <si>
+    <t>tư</t>
+  </si>
+  <si>
+    <t>tư liệu, vốn</t>
+  </si>
+  <si>
+    <t>nhẫn</t>
+  </si>
+  <si>
+    <t>tiền công</t>
+  </si>
+  <si>
+    <t>tán</t>
+  </si>
+  <si>
+    <t>tán thành</t>
+  </si>
+  <si>
+    <t>chất</t>
+  </si>
+  <si>
+    <t>chất vấn</t>
+  </si>
+  <si>
+    <t>thưởng</t>
+  </si>
+  <si>
+    <t>giải thưởng</t>
+  </si>
+  <si>
+    <t>tặng</t>
+  </si>
+  <si>
+    <t>関</t>
+  </si>
+  <si>
+    <t>集</t>
+  </si>
+  <si>
+    <t>離</t>
+  </si>
+  <si>
+    <t>雲</t>
+  </si>
+  <si>
+    <t>震</t>
+  </si>
+  <si>
+    <t>非</t>
+  </si>
+  <si>
+    <t>面</t>
+  </si>
+  <si>
+    <t>預</t>
+  </si>
+  <si>
+    <t>頑</t>
+  </si>
+  <si>
+    <t>額</t>
+  </si>
+  <si>
+    <t>類</t>
+  </si>
+  <si>
+    <t>願</t>
+  </si>
+  <si>
+    <t>飛</t>
+  </si>
+  <si>
+    <t>飾</t>
+  </si>
+  <si>
+    <t>駐</t>
+  </si>
+  <si>
+    <t>騷</t>
+  </si>
+  <si>
+    <t>髮</t>
+  </si>
+  <si>
+    <t>黃</t>
+  </si>
+  <si>
+    <t>歯</t>
+  </si>
+  <si>
+    <t>việt</t>
+  </si>
+  <si>
+    <t>vượt qua</t>
+  </si>
+  <si>
+    <t>thú</t>
+  </si>
+  <si>
+    <t>thú vui</t>
+  </si>
+  <si>
+    <t>dũng</t>
+  </si>
+  <si>
+    <t>nhảy múa</t>
+  </si>
+  <si>
+    <t>đạp</t>
+  </si>
+  <si>
+    <t>giẫm đạp</t>
+  </si>
+  <si>
+    <t>thân</t>
+  </si>
+  <si>
+    <t>cơ thể</t>
+  </si>
+  <si>
+    <t>thâu</t>
+  </si>
+  <si>
+    <t>chuyên chở</t>
+  </si>
+  <si>
+    <t>nông</t>
+  </si>
+  <si>
+    <t>nông nghiệp</t>
+  </si>
+  <si>
+    <t>tuý</t>
+  </si>
+  <si>
+    <t>say rượu</t>
+  </si>
+  <si>
+    <t>dã</t>
+  </si>
+  <si>
+    <t>hoang dã</t>
+  </si>
+  <si>
+    <t>lượng</t>
+  </si>
+  <si>
+    <t>số lượng</t>
+  </si>
+  <si>
+    <t>mạch</t>
+  </si>
+  <si>
+    <t>lúa mạch, lúa mạch</t>
+  </si>
+  <si>
+    <t>thiết</t>
+  </si>
+  <si>
+    <t>sắt</t>
+  </si>
+  <si>
+    <t>duyên</t>
+  </si>
+  <si>
+    <t>chất chì</t>
+  </si>
+  <si>
+    <t>quan</t>
+  </si>
+  <si>
+    <t>tập</t>
+  </si>
+  <si>
+    <t>tập hợp</t>
+  </si>
+  <si>
+    <t>ly</t>
+  </si>
+  <si>
+    <t>rời xa</t>
+  </si>
+  <si>
+    <t>vân</t>
+  </si>
+  <si>
+    <t>mây</t>
+  </si>
+  <si>
+    <t>chấn</t>
+  </si>
+  <si>
+    <t>địa chấn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phi </t>
+  </si>
+  <si>
+    <t>phi thường</t>
+  </si>
+  <si>
+    <t>diện</t>
+  </si>
+  <si>
+    <t>bề mặt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dư </t>
+  </si>
+  <si>
+    <t xml:space="preserve">gửi </t>
+  </si>
+  <si>
+    <t>ngoan</t>
+  </si>
+  <si>
+    <t>bướn bỉnh</t>
+  </si>
+  <si>
+    <t>ngạch</t>
+  </si>
+  <si>
+    <t>hạn ngạch</t>
+  </si>
+  <si>
+    <t>loại</t>
+  </si>
+  <si>
+    <t>nhà ga</t>
+  </si>
+  <si>
+    <t xml:space="preserve">trú </t>
+  </si>
+  <si>
+    <t>dừng</t>
+  </si>
+  <si>
+    <t>nguyện</t>
+  </si>
+  <si>
+    <t>nhờ</t>
+  </si>
+  <si>
+    <t>trú</t>
+  </si>
+  <si>
+    <t>tao</t>
+  </si>
+  <si>
+    <t>làm ổn</t>
+  </si>
+  <si>
+    <t>phát</t>
+  </si>
+  <si>
+    <t>tóc</t>
+  </si>
+  <si>
+    <t>hoàng</t>
+  </si>
+  <si>
+    <t>màu vàng</t>
+  </si>
+  <si>
+    <t>xỉ</t>
+  </si>
+  <si>
+    <t>răng</t>
+  </si>
+  <si>
+    <t>齡</t>
+  </si>
+  <si>
+    <t>linh</t>
+  </si>
+  <si>
+    <t>tuổi tác</t>
+  </si>
+  <si>
+    <t>録</t>
+  </si>
+  <si>
+    <t>ghi chép</t>
   </si>
 </sst>
 </file>
@@ -1750,7 +3178,14 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -2032,16 +3467,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D366"/>
+  <dimension ref="A1:D376"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A325" workbookViewId="0">
+      <selection activeCell="H336" sqref="H336"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -4151,29 +5586,1898 @@
         <v>550</v>
       </c>
     </row>
-    <row r="203" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B203" s="4"/>
-    </row>
-    <row r="206" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B206" s="4"/>
-    </row>
-    <row r="255" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B255" s="2"/>
-    </row>
-    <row r="306" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B306" s="2"/>
-    </row>
-    <row r="315" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B315" s="2"/>
-    </row>
-    <row r="355" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B355" s="2"/>
-    </row>
-    <row r="366" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B366" s="2"/>
+    <row r="192" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B192" t="s">
+        <v>552</v>
+      </c>
+      <c r="C192" t="s">
+        <v>553</v>
+      </c>
+      <c r="D192" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="193" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B193" t="s">
+        <v>554</v>
+      </c>
+      <c r="C193" t="s">
+        <v>555</v>
+      </c>
+      <c r="D193" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="194" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B194" t="s">
+        <v>557</v>
+      </c>
+      <c r="C194" t="s">
+        <v>558</v>
+      </c>
+      <c r="D194" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="195" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B195" t="s">
+        <v>560</v>
+      </c>
+      <c r="C195" t="s">
+        <v>561</v>
+      </c>
+      <c r="D195" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="196" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B196" t="s">
+        <v>563</v>
+      </c>
+      <c r="C196" t="s">
+        <v>564</v>
+      </c>
+      <c r="D196" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="197" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B197" t="s">
+        <v>566</v>
+      </c>
+      <c r="C197" t="s">
+        <v>30</v>
+      </c>
+      <c r="D197" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="198" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B198" t="s">
+        <v>568</v>
+      </c>
+      <c r="C198" t="s">
+        <v>569</v>
+      </c>
+      <c r="D198" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="199" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B199" t="s">
+        <v>571</v>
+      </c>
+      <c r="C199" t="s">
+        <v>574</v>
+      </c>
+      <c r="D199" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="200" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B200" t="s">
+        <v>572</v>
+      </c>
+      <c r="C200" t="s">
+        <v>576</v>
+      </c>
+      <c r="D200" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="201" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B201" t="s">
+        <v>573</v>
+      </c>
+      <c r="C201" t="s">
+        <v>578</v>
+      </c>
+      <c r="D201" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="202" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B202" t="s">
+        <v>580</v>
+      </c>
+      <c r="C202" t="s">
+        <v>581</v>
+      </c>
+      <c r="D202" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="203" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B203" s="4" t="s">
+        <v>583</v>
+      </c>
+      <c r="C203" t="s">
+        <v>584</v>
+      </c>
+      <c r="D203" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="204" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B204" t="s">
+        <v>585</v>
+      </c>
+      <c r="C204" t="s">
+        <v>586</v>
+      </c>
+      <c r="D204" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="205" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B205" t="s">
+        <v>588</v>
+      </c>
+      <c r="C205" t="s">
+        <v>589</v>
+      </c>
+      <c r="D205" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="206" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B206" s="4" t="s">
+        <v>591</v>
+      </c>
+      <c r="C206" t="s">
+        <v>592</v>
+      </c>
+      <c r="D206" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="207" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B207" t="s">
+        <v>594</v>
+      </c>
+      <c r="C207" t="s">
+        <v>595</v>
+      </c>
+      <c r="D207" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="208" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B208" t="s">
+        <v>597</v>
+      </c>
+      <c r="C208" t="s">
+        <v>599</v>
+      </c>
+      <c r="D208" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="209" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B209" t="s">
+        <v>598</v>
+      </c>
+      <c r="C209" t="s">
+        <v>601</v>
+      </c>
+      <c r="D209" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="210" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B210" t="s">
+        <v>603</v>
+      </c>
+      <c r="C210" t="s">
+        <v>605</v>
+      </c>
+      <c r="D210" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="211" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B211" t="s">
+        <v>604</v>
+      </c>
+      <c r="C211" t="s">
+        <v>607</v>
+      </c>
+      <c r="D211" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="212" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B212" t="s">
+        <v>609</v>
+      </c>
+      <c r="C212" t="s">
+        <v>616</v>
+      </c>
+      <c r="D212" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="213" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B213" t="s">
+        <v>610</v>
+      </c>
+      <c r="C213" t="s">
+        <v>618</v>
+      </c>
+      <c r="D213" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="214" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B214" t="s">
+        <v>611</v>
+      </c>
+      <c r="C214" t="s">
+        <v>75</v>
+      </c>
+      <c r="D214" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="215" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B215" t="s">
+        <v>612</v>
+      </c>
+      <c r="C215" t="s">
+        <v>621</v>
+      </c>
+      <c r="D215" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="216" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B216" t="s">
+        <v>613</v>
+      </c>
+      <c r="C216" t="s">
+        <v>623</v>
+      </c>
+      <c r="D216" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="217" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B217" t="s">
+        <v>614</v>
+      </c>
+      <c r="C217" t="s">
+        <v>625</v>
+      </c>
+      <c r="D217" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="218" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B218" t="s">
+        <v>615</v>
+      </c>
+      <c r="C218" t="s">
+        <v>627</v>
+      </c>
+      <c r="D218" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="219" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B219" t="s">
+        <v>629</v>
+      </c>
+      <c r="C219" t="s">
+        <v>393</v>
+      </c>
+      <c r="D219" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="220" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B220" t="s">
+        <v>630</v>
+      </c>
+      <c r="C220" t="s">
+        <v>633</v>
+      </c>
+      <c r="D220" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="221" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B221" t="s">
+        <v>631</v>
+      </c>
+      <c r="C221" t="s">
+        <v>26</v>
+      </c>
+      <c r="D221" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="222" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B222" t="s">
+        <v>636</v>
+      </c>
+      <c r="C222" t="s">
+        <v>643</v>
+      </c>
+      <c r="D222" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="223" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B223" t="s">
+        <v>637</v>
+      </c>
+      <c r="C223" t="s">
+        <v>66</v>
+      </c>
+      <c r="D223" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="224" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B224" t="s">
+        <v>638</v>
+      </c>
+      <c r="C224" t="s">
+        <v>646</v>
+      </c>
+      <c r="D224" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="225" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B225" t="s">
+        <v>639</v>
+      </c>
+      <c r="C225" t="s">
+        <v>647</v>
+      </c>
+      <c r="D225" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="226" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B226" t="s">
+        <v>640</v>
+      </c>
+      <c r="C226" t="s">
+        <v>649</v>
+      </c>
+      <c r="D226" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="227" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B227" t="s">
+        <v>641</v>
+      </c>
+      <c r="C227" t="s">
+        <v>651</v>
+      </c>
+      <c r="D227" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="228" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B228" t="s">
+        <v>642</v>
+      </c>
+      <c r="C228" t="s">
+        <v>165</v>
+      </c>
+      <c r="D228" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="229" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B229" t="s">
+        <v>654</v>
+      </c>
+      <c r="C229" t="s">
+        <v>657</v>
+      </c>
+      <c r="D229" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="230" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B230" t="s">
+        <v>655</v>
+      </c>
+      <c r="C230" t="s">
+        <v>658</v>
+      </c>
+      <c r="D230" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="231" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B231" t="s">
+        <v>656</v>
+      </c>
+      <c r="C231" t="s">
+        <v>660</v>
+      </c>
+      <c r="D231" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="232" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B232" t="s">
+        <v>663</v>
+      </c>
+      <c r="C232" t="s">
+        <v>668</v>
+      </c>
+      <c r="D232" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="233" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B233" t="s">
+        <v>664</v>
+      </c>
+      <c r="C233" t="s">
+        <v>670</v>
+      </c>
+      <c r="D233" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="234" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B234" t="s">
+        <v>665</v>
+      </c>
+      <c r="C234" t="s">
+        <v>672</v>
+      </c>
+      <c r="D234" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="235" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B235" t="s">
+        <v>666</v>
+      </c>
+      <c r="C235" t="s">
+        <v>674</v>
+      </c>
+      <c r="D235" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="236" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B236" t="s">
+        <v>667</v>
+      </c>
+      <c r="C236" t="s">
+        <v>676</v>
+      </c>
+      <c r="D236" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="237" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B237" t="s">
+        <v>678</v>
+      </c>
+      <c r="C237" t="s">
+        <v>683</v>
+      </c>
+      <c r="D237" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="238" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B238" t="s">
+        <v>679</v>
+      </c>
+      <c r="C238" t="s">
+        <v>672</v>
+      </c>
+      <c r="D238" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="239" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B239" t="s">
+        <v>680</v>
+      </c>
+      <c r="C239" t="s">
+        <v>686</v>
+      </c>
+      <c r="D239" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="240" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B240" t="s">
+        <v>681</v>
+      </c>
+      <c r="C240" t="s">
+        <v>688</v>
+      </c>
+      <c r="D240" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="241" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B241" t="s">
+        <v>682</v>
+      </c>
+      <c r="C241" t="s">
+        <v>690</v>
+      </c>
+      <c r="D241" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="242" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B242" t="s">
+        <v>692</v>
+      </c>
+      <c r="C242" t="s">
+        <v>699</v>
+      </c>
+      <c r="D242" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="243" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B243" t="s">
+        <v>693</v>
+      </c>
+      <c r="C243" t="s">
+        <v>701</v>
+      </c>
+      <c r="D243" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="244" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B244" t="s">
+        <v>694</v>
+      </c>
+      <c r="C244" t="s">
+        <v>703</v>
+      </c>
+      <c r="D244" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="245" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B245" t="s">
+        <v>695</v>
+      </c>
+      <c r="C245" t="s">
+        <v>705</v>
+      </c>
+      <c r="D245" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="246" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B246" t="s">
+        <v>696</v>
+      </c>
+      <c r="C246" t="s">
+        <v>707</v>
+      </c>
+      <c r="D246" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="247" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B247" t="s">
+        <v>697</v>
+      </c>
+      <c r="C247" t="s">
+        <v>211</v>
+      </c>
+      <c r="D247" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="248" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B248" t="s">
+        <v>698</v>
+      </c>
+      <c r="C248" t="s">
+        <v>710</v>
+      </c>
+      <c r="D248" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="249" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B249" t="s">
+        <v>712</v>
+      </c>
+      <c r="C249" t="s">
+        <v>715</v>
+      </c>
+      <c r="D249" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="250" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B250" t="s">
+        <v>713</v>
+      </c>
+      <c r="C250" t="s">
+        <v>717</v>
+      </c>
+      <c r="D250" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="251" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B251" t="s">
+        <v>714</v>
+      </c>
+      <c r="C251" t="s">
+        <v>546</v>
+      </c>
+      <c r="D251" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="252" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B252" t="s">
+        <v>720</v>
+      </c>
+      <c r="C252" t="s">
+        <v>725</v>
+      </c>
+      <c r="D252" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="253" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B253" t="s">
+        <v>721</v>
+      </c>
+      <c r="C253" t="s">
+        <v>727</v>
+      </c>
+      <c r="D253" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="254" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B254" t="s">
+        <v>722</v>
+      </c>
+      <c r="C254" t="s">
+        <v>729</v>
+      </c>
+      <c r="D254" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="255" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B255" s="2" t="s">
+        <v>723</v>
+      </c>
+      <c r="C255" t="s">
+        <v>731</v>
+      </c>
+      <c r="D255" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="256" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B256" t="s">
+        <v>733</v>
+      </c>
+      <c r="C256" t="s">
+        <v>734</v>
+      </c>
+      <c r="D256" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="257" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B257" t="s">
+        <v>724</v>
+      </c>
+      <c r="C257" t="s">
+        <v>736</v>
+      </c>
+      <c r="D257" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="258" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B258" t="s">
+        <v>788</v>
+      </c>
+      <c r="C258" t="s">
+        <v>514</v>
+      </c>
+      <c r="D258" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="259" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B259" t="s">
+        <v>789</v>
+      </c>
+      <c r="C259" t="s">
+        <v>793</v>
+      </c>
+      <c r="D259" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="260" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B260" t="s">
+        <v>790</v>
+      </c>
+      <c r="C260" t="s">
+        <v>795</v>
+      </c>
+      <c r="D260" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="261" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B261" t="s">
+        <v>791</v>
+      </c>
+      <c r="C261" t="s">
+        <v>757</v>
+      </c>
+      <c r="D261" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="262" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B262" t="s">
+        <v>738</v>
+      </c>
+      <c r="C262" t="s">
+        <v>745</v>
+      </c>
+      <c r="D262" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="263" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B263" t="s">
+        <v>739</v>
+      </c>
+      <c r="C263" t="s">
+        <v>747</v>
+      </c>
+      <c r="D263" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="264" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B264" t="s">
+        <v>740</v>
+      </c>
+      <c r="C264" t="s">
+        <v>749</v>
+      </c>
+      <c r="D264" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="265" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B265" t="s">
+        <v>741</v>
+      </c>
+      <c r="C265" t="s">
+        <v>751</v>
+      </c>
+      <c r="D265" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="266" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B266" t="s">
+        <v>742</v>
+      </c>
+      <c r="C266" t="s">
+        <v>753</v>
+      </c>
+      <c r="D266" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="267" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B267" t="s">
+        <v>743</v>
+      </c>
+      <c r="C267" t="s">
+        <v>755</v>
+      </c>
+      <c r="D267" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="268" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B268" t="s">
+        <v>744</v>
+      </c>
+      <c r="C268" t="s">
+        <v>757</v>
+      </c>
+      <c r="D268" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="269" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B269" t="s">
+        <v>765</v>
+      </c>
+      <c r="C269" t="s">
+        <v>768</v>
+      </c>
+      <c r="D269" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="270" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B270" t="s">
+        <v>766</v>
+      </c>
+      <c r="C270" t="s">
+        <v>769</v>
+      </c>
+      <c r="D270" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="271" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B271" t="s">
+        <v>767</v>
+      </c>
+      <c r="C271" t="s">
+        <v>771</v>
+      </c>
+      <c r="D271" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="272" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B272" t="s">
+        <v>759</v>
+      </c>
+      <c r="C272" t="s">
+        <v>29</v>
+      </c>
+      <c r="D272" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="273" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B273" t="s">
+        <v>760</v>
+      </c>
+      <c r="C273" t="s">
+        <v>727</v>
+      </c>
+      <c r="D273" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="274" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B274" t="s">
+        <v>798</v>
+      </c>
+      <c r="C274" t="s">
+        <v>799</v>
+      </c>
+      <c r="D274" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="275" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B275" t="s">
+        <v>761</v>
+      </c>
+      <c r="C275" t="s">
+        <v>771</v>
+      </c>
+      <c r="D275" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="276" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B276" t="s">
+        <v>762</v>
+      </c>
+      <c r="C276" t="s">
+        <v>775</v>
+      </c>
+      <c r="D276" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="277" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B277" t="s">
+        <v>763</v>
+      </c>
+      <c r="C277" t="s">
+        <v>33</v>
+      </c>
+      <c r="D277" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="278" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B278" t="s">
+        <v>764</v>
+      </c>
+      <c r="C278" t="s">
+        <v>777</v>
+      </c>
+      <c r="D278" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="279" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B279" t="s">
+        <v>779</v>
+      </c>
+      <c r="C279" t="s">
+        <v>782</v>
+      </c>
+      <c r="D279" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="280" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B280" t="s">
+        <v>780</v>
+      </c>
+      <c r="C280" t="s">
+        <v>784</v>
+      </c>
+      <c r="D280" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="281" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B281" t="s">
+        <v>781</v>
+      </c>
+      <c r="C281" t="s">
+        <v>786</v>
+      </c>
+      <c r="D281" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="282" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B282" t="s">
+        <v>801</v>
+      </c>
+      <c r="C282" t="s">
+        <v>810</v>
+      </c>
+      <c r="D282" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="283" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B283" t="s">
+        <v>802</v>
+      </c>
+      <c r="C283" t="s">
+        <v>812</v>
+      </c>
+      <c r="D283" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="284" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B284" t="s">
+        <v>803</v>
+      </c>
+      <c r="C284" t="s">
+        <v>814</v>
+      </c>
+      <c r="D284" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="285" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B285" t="s">
+        <v>804</v>
+      </c>
+      <c r="C285" t="s">
+        <v>54</v>
+      </c>
+      <c r="D285" t="s">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="286" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B286" t="s">
+        <v>805</v>
+      </c>
+      <c r="C286" t="s">
+        <v>816</v>
+      </c>
+      <c r="D286" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="287" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B287" t="s">
+        <v>806</v>
+      </c>
+      <c r="C287" t="s">
+        <v>818</v>
+      </c>
+      <c r="D287" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="288" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B288" t="s">
+        <v>826</v>
+      </c>
+      <c r="C288" t="s">
+        <v>827</v>
+      </c>
+      <c r="D288" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="289" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B289" t="s">
+        <v>807</v>
+      </c>
+      <c r="C289" t="s">
+        <v>820</v>
+      </c>
+      <c r="D289" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="290" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B290" t="s">
+        <v>808</v>
+      </c>
+      <c r="C290" t="s">
+        <v>822</v>
+      </c>
+      <c r="D290" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="291" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B291" t="s">
+        <v>809</v>
+      </c>
+      <c r="C291" t="s">
+        <v>823</v>
+      </c>
+      <c r="D291" t="s">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="292" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B292" t="s">
+        <v>829</v>
+      </c>
+      <c r="C292" t="s">
+        <v>839</v>
+      </c>
+      <c r="D292" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="293" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B293" t="s">
+        <v>830</v>
+      </c>
+      <c r="C293" t="s">
+        <v>40</v>
+      </c>
+      <c r="D293" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="294" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B294" t="s">
+        <v>831</v>
+      </c>
+      <c r="C294" t="s">
+        <v>842</v>
+      </c>
+      <c r="D294" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="295" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B295" t="s">
+        <v>832</v>
+      </c>
+      <c r="C295" t="s">
+        <v>844</v>
+      </c>
+      <c r="D295" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="296" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B296" t="s">
+        <v>833</v>
+      </c>
+      <c r="C296" t="s">
+        <v>846</v>
+      </c>
+      <c r="D296" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="297" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B297" t="s">
+        <v>834</v>
+      </c>
+      <c r="C297" t="s">
+        <v>848</v>
+      </c>
+      <c r="D297" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="298" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B298" t="s">
+        <v>835</v>
+      </c>
+      <c r="C298" t="s">
+        <v>849</v>
+      </c>
+      <c r="D298" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="299" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B299" t="s">
+        <v>836</v>
+      </c>
+      <c r="C299" t="s">
+        <v>851</v>
+      </c>
+      <c r="D299" t="s">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="300" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B300" t="s">
+        <v>837</v>
+      </c>
+      <c r="C300" t="s">
+        <v>853</v>
+      </c>
+      <c r="D300" t="s">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="301" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B301" t="s">
+        <v>838</v>
+      </c>
+      <c r="C301" t="s">
+        <v>849</v>
+      </c>
+      <c r="D301" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="302" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B302" t="s">
+        <v>856</v>
+      </c>
+      <c r="C302" t="s">
+        <v>860</v>
+      </c>
+      <c r="D302" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="303" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B303" t="s">
+        <v>857</v>
+      </c>
+      <c r="C303" t="s">
+        <v>862</v>
+      </c>
+      <c r="D303" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="304" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B304" t="s">
+        <v>858</v>
+      </c>
+      <c r="C304" t="s">
+        <v>15</v>
+      </c>
+      <c r="D304" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="305" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B305" t="s">
+        <v>859</v>
+      </c>
+      <c r="C305" t="s">
+        <v>865</v>
+      </c>
+      <c r="D305" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="306" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B306" t="s">
+        <v>867</v>
+      </c>
+      <c r="C306" t="s">
+        <v>873</v>
+      </c>
+      <c r="D306" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="307" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B307" t="s">
+        <v>868</v>
+      </c>
+      <c r="C307" t="s">
+        <v>875</v>
+      </c>
+      <c r="D307" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="308" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B308" t="s">
+        <v>869</v>
+      </c>
+      <c r="C308" t="s">
+        <v>877</v>
+      </c>
+      <c r="D308" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="309" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B309" t="s">
+        <v>870</v>
+      </c>
+      <c r="C309" t="s">
+        <v>879</v>
+      </c>
+      <c r="D309" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="310" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B310" t="s">
+        <v>871</v>
+      </c>
+      <c r="C310" t="s">
+        <v>881</v>
+      </c>
+      <c r="D310" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="311" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B311" s="2" t="s">
+        <v>872</v>
+      </c>
+      <c r="C311" t="s">
+        <v>883</v>
+      </c>
+      <c r="D311" t="s">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="312" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B312" t="s">
+        <v>885</v>
+      </c>
+      <c r="C312" t="s">
+        <v>895</v>
+      </c>
+      <c r="D312" t="s">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="313" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B313" t="s">
+        <v>886</v>
+      </c>
+      <c r="C313" t="s">
+        <v>897</v>
+      </c>
+      <c r="D313" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="314" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B314" t="s">
+        <v>887</v>
+      </c>
+      <c r="C314" t="s">
+        <v>899</v>
+      </c>
+      <c r="D314" t="s">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="315" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B315" t="s">
+        <v>888</v>
+      </c>
+      <c r="C315" t="s">
+        <v>524</v>
+      </c>
+      <c r="D315" t="s">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="316" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B316" t="s">
+        <v>889</v>
+      </c>
+      <c r="C316" t="s">
+        <v>901</v>
+      </c>
+      <c r="D316" t="s">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="317" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B317" t="s">
+        <v>890</v>
+      </c>
+      <c r="C317" t="s">
+        <v>903</v>
+      </c>
+      <c r="D317" t="s">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="318" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B318" t="s">
+        <v>891</v>
+      </c>
+      <c r="C318" t="s">
+        <v>905</v>
+      </c>
+      <c r="D318" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="319" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B319" t="s">
+        <v>892</v>
+      </c>
+      <c r="C319" t="s">
+        <v>907</v>
+      </c>
+      <c r="D319" t="s">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="320" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B320" t="s">
+        <v>893</v>
+      </c>
+      <c r="C320" t="s">
+        <v>633</v>
+      </c>
+      <c r="D320" t="s">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="321" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B321" t="s">
+        <v>894</v>
+      </c>
+      <c r="C321" t="s">
+        <v>910</v>
+      </c>
+      <c r="D321" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="322" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B322" t="s">
+        <v>913</v>
+      </c>
+      <c r="C322" t="s">
+        <v>933</v>
+      </c>
+      <c r="D322" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="323" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B323" t="s">
+        <v>914</v>
+      </c>
+      <c r="C323" t="s">
+        <v>935</v>
+      </c>
+      <c r="D323" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="324" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B324" s="2" t="s">
+        <v>915</v>
+      </c>
+      <c r="C324" t="s">
+        <v>937</v>
+      </c>
+      <c r="D324" t="s">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="325" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B325" t="s">
+        <v>916</v>
+      </c>
+      <c r="C325" t="s">
+        <v>939</v>
+      </c>
+      <c r="D325" t="s">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="326" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B326" t="s">
+        <v>921</v>
+      </c>
+      <c r="C326" t="s">
+        <v>941</v>
+      </c>
+      <c r="D326" t="s">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="327" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B327" t="s">
+        <v>922</v>
+      </c>
+      <c r="C327" t="s">
+        <v>943</v>
+      </c>
+      <c r="D327" t="s">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="328" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B328" t="s">
+        <v>923</v>
+      </c>
+      <c r="C328" t="s">
+        <v>963</v>
+      </c>
+      <c r="D328" t="s">
+        <v>964</v>
+      </c>
+    </row>
+    <row r="329" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B329" t="s">
+        <v>924</v>
+      </c>
+      <c r="C329" t="s">
+        <v>965</v>
+      </c>
+      <c r="D329" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="330" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B330" t="s">
+        <v>926</v>
+      </c>
+      <c r="C330" t="s">
+        <v>967</v>
+      </c>
+      <c r="D330" t="s">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="331" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B331" t="s">
+        <v>927</v>
+      </c>
+      <c r="C331" t="s">
+        <v>969</v>
+      </c>
+      <c r="D331" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="332" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B332" t="s">
+        <v>928</v>
+      </c>
+      <c r="C332" t="s">
+        <v>971</v>
+      </c>
+      <c r="D332" t="s">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="333" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B333" t="s">
+        <v>929</v>
+      </c>
+      <c r="C333" t="s">
+        <v>973</v>
+      </c>
+      <c r="D333" t="s">
+        <v>974</v>
+      </c>
+    </row>
+    <row r="334" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B334" t="s">
+        <v>917</v>
+      </c>
+      <c r="C334" t="s">
+        <v>975</v>
+      </c>
+      <c r="D334" t="s">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="335" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B335" t="s">
+        <v>918</v>
+      </c>
+      <c r="C335" t="s">
+        <v>977</v>
+      </c>
+      <c r="D335" t="s">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="336" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B336" t="s">
+        <v>919</v>
+      </c>
+      <c r="C336" t="s">
+        <v>979</v>
+      </c>
+      <c r="D336" t="s">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="337" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B337" t="s">
+        <v>920</v>
+      </c>
+      <c r="C337" t="s">
+        <v>981</v>
+      </c>
+      <c r="D337" t="s">
+        <v>982</v>
+      </c>
+    </row>
+    <row r="338" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B338" t="s">
+        <v>925</v>
+      </c>
+      <c r="C338" t="s">
+        <v>20</v>
+      </c>
+      <c r="D338" t="s">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="339" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B339" t="s">
+        <v>930</v>
+      </c>
+      <c r="C339" t="s">
+        <v>983</v>
+      </c>
+      <c r="D339" t="s">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="340" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B340" t="s">
+        <v>1026</v>
+      </c>
+      <c r="C340" t="s">
+        <v>782</v>
+      </c>
+      <c r="D340" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="341" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B341" t="s">
+        <v>931</v>
+      </c>
+      <c r="C341" t="s">
+        <v>985</v>
+      </c>
+      <c r="D341" t="s">
+        <v>986</v>
+      </c>
+    </row>
+    <row r="342" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B342" t="s">
+        <v>932</v>
+      </c>
+      <c r="C342" t="s">
+        <v>987</v>
+      </c>
+      <c r="D342" t="s">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="343" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B343" t="s">
+        <v>944</v>
+      </c>
+      <c r="C343" t="s">
+        <v>989</v>
+      </c>
+      <c r="D343" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="344" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B344" t="s">
+        <v>945</v>
+      </c>
+      <c r="C344" t="s">
+        <v>990</v>
+      </c>
+      <c r="D344" t="s">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="345" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B345" t="s">
+        <v>946</v>
+      </c>
+      <c r="C345" t="s">
+        <v>992</v>
+      </c>
+      <c r="D345" t="s">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="346" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B346" t="s">
+        <v>947</v>
+      </c>
+      <c r="C346" t="s">
+        <v>994</v>
+      </c>
+      <c r="D346" t="s">
+        <v>995</v>
+      </c>
+    </row>
+    <row r="347" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B347" t="s">
+        <v>948</v>
+      </c>
+      <c r="C347" t="s">
+        <v>996</v>
+      </c>
+      <c r="D347" t="s">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="348" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B348" t="s">
+        <v>949</v>
+      </c>
+      <c r="C348" t="s">
+        <v>998</v>
+      </c>
+      <c r="D348" t="s">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="349" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B349" t="s">
+        <v>950</v>
+      </c>
+      <c r="C349" t="s">
+        <v>1000</v>
+      </c>
+      <c r="D349" t="s">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="350" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B350" t="s">
+        <v>951</v>
+      </c>
+      <c r="C350" t="s">
+        <v>1002</v>
+      </c>
+      <c r="D350" t="s">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="351" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B351" t="s">
+        <v>952</v>
+      </c>
+      <c r="C351" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D351" t="s">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="352" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B352" t="s">
+        <v>953</v>
+      </c>
+      <c r="C352" t="s">
+        <v>1006</v>
+      </c>
+      <c r="D352" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="353" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B353" t="s">
+        <v>954</v>
+      </c>
+      <c r="C353" t="s">
+        <v>1008</v>
+      </c>
+      <c r="D353" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="354" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B354" t="s">
+        <v>955</v>
+      </c>
+      <c r="C354" t="s">
+        <v>15</v>
+      </c>
+      <c r="D354" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="355" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B355" t="s">
+        <v>956</v>
+      </c>
+      <c r="C355" t="s">
+        <v>1010</v>
+      </c>
+      <c r="D355" t="s">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="356" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B356" t="s">
+        <v>957</v>
+      </c>
+      <c r="C356" t="s">
+        <v>1012</v>
+      </c>
+      <c r="D356" t="s">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="357" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B357" t="s">
+        <v>958</v>
+      </c>
+      <c r="C357" t="s">
+        <v>1014</v>
+      </c>
+      <c r="D357" t="s">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="358" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B358" t="s">
+        <v>959</v>
+      </c>
+      <c r="C358" t="s">
+        <v>1015</v>
+      </c>
+      <c r="D358" t="s">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="359" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B359" t="s">
+        <v>960</v>
+      </c>
+      <c r="C359" t="s">
+        <v>1017</v>
+      </c>
+      <c r="D359" t="s">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="360" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B360" t="s">
+        <v>961</v>
+      </c>
+      <c r="C360" t="s">
+        <v>1019</v>
+      </c>
+      <c r="D360" t="s">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="361" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B361" t="s">
+        <v>962</v>
+      </c>
+      <c r="C361" t="s">
+        <v>1021</v>
+      </c>
+      <c r="D361" t="s">
+        <v>1022</v>
+      </c>
+    </row>
+    <row r="362" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B362" t="s">
+        <v>1023</v>
+      </c>
+      <c r="C362" t="s">
+        <v>1024</v>
+      </c>
+      <c r="D362" t="s">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="365" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B365" s="2"/>
+    </row>
+    <row r="376" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B376" s="2"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B52">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B316:B1048576 B293:B311 B280:B291 B1:B278">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add lesson 13 tuvung
</commit_message>
<xml_diff>
--- a/Review_Kanji_V2/Lesson2/kanjiv2.xlsx
+++ b/Review_Kanji_V2/Lesson2/kanjiv2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\01_LearningJapaneseWebProject\Review_Kanji_V2\Lesson2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CE6FA15-4FFF-49B9-98A0-40E59C5A8525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63495E7F-6066-4809-80FC-A9A4E6F08800}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9240" yWindow="1815" windowWidth="21495" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3469,8 +3469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D376"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A325" workbookViewId="0">
-      <selection activeCell="H336" sqref="H336"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3872,24 +3872,24 @@
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="C36" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="D36" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>132</v>
+        <v>147</v>
       </c>
       <c r="C37" t="s">
-        <v>133</v>
+        <v>148</v>
       </c>
       <c r="D37" t="s">
-        <v>134</v>
+        <v>149</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.25">
@@ -7475,10 +7475,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B52">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B316:B1048576 B293:B311 B280:B291 B1:B278">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="7"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add lesson 15 tuvung
</commit_message>
<xml_diff>
--- a/Review_Kanji_V2/Lesson2/kanjiv2.xlsx
+++ b/Review_Kanji_V2/Lesson2/kanjiv2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\01_LearningJapaneseWebProject\Review_Kanji_V2\Lesson2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63495E7F-6066-4809-80FC-A9A4E6F08800}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8DAFE5D-6522-4B05-A711-3EFD86F658B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1088" uniqueCount="1028">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1118" uniqueCount="1056">
   <si>
     <t>japanese</t>
   </si>
@@ -3109,6 +3109,90 @@
   </si>
   <si>
     <t>ghi chép</t>
+  </si>
+  <si>
+    <t>障</t>
+  </si>
+  <si>
+    <t>隣</t>
+  </si>
+  <si>
+    <t>必</t>
+  </si>
+  <si>
+    <t>応</t>
+  </si>
+  <si>
+    <t>急</t>
+  </si>
+  <si>
+    <t>怒</t>
+  </si>
+  <si>
+    <t>怖</t>
+  </si>
+  <si>
+    <t>息</t>
+  </si>
+  <si>
+    <t>恥</t>
+  </si>
+  <si>
+    <t>情</t>
+  </si>
+  <si>
+    <t>chướng</t>
+  </si>
+  <si>
+    <t>cố chướng</t>
+  </si>
+  <si>
+    <t>lân</t>
+  </si>
+  <si>
+    <t>bên cạnh</t>
+  </si>
+  <si>
+    <t>tất</t>
+  </si>
+  <si>
+    <t>tất yếu</t>
+  </si>
+  <si>
+    <t>ứng</t>
+  </si>
+  <si>
+    <t>phản ứng</t>
+  </si>
+  <si>
+    <t>vội vàng</t>
+  </si>
+  <si>
+    <t>nộ</t>
+  </si>
+  <si>
+    <t>bực tức</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bố </t>
+  </si>
+  <si>
+    <t>sợ hãi, dữ</t>
+  </si>
+  <si>
+    <t>tức</t>
+  </si>
+  <si>
+    <t>hơi thở</t>
+  </si>
+  <si>
+    <t>sỉ</t>
+  </si>
+  <si>
+    <t>mắc cỡ</t>
+  </si>
+  <si>
+    <t>tình cảm</t>
   </si>
 </sst>
 </file>
@@ -3467,10 +3551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D376"/>
+  <dimension ref="A1:D386"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="F156" sqref="F156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5148,2336 +5232,2446 @@
     </row>
     <row r="152" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B152" t="s">
-        <v>450</v>
+        <v>1028</v>
       </c>
       <c r="C152" t="s">
-        <v>460</v>
+        <v>1038</v>
       </c>
       <c r="D152" t="s">
-        <v>461</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="153" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B153" t="s">
-        <v>451</v>
+        <v>1029</v>
       </c>
       <c r="C153" t="s">
-        <v>462</v>
+        <v>1040</v>
       </c>
       <c r="D153" t="s">
-        <v>12</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="154" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B154" t="s">
-        <v>452</v>
+        <v>1030</v>
       </c>
       <c r="C154" t="s">
-        <v>463</v>
+        <v>1042</v>
       </c>
       <c r="D154" t="s">
-        <v>464</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="155" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B155" t="s">
-        <v>453</v>
+        <v>1031</v>
       </c>
       <c r="C155" t="s">
-        <v>465</v>
+        <v>1044</v>
       </c>
       <c r="D155" t="s">
-        <v>466</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="156" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B156" t="s">
-        <v>454</v>
+        <v>1032</v>
       </c>
       <c r="C156" t="s">
-        <v>17</v>
+        <v>771</v>
       </c>
       <c r="D156" t="s">
-        <v>468</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="157" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B157" t="s">
-        <v>455</v>
+        <v>1033</v>
       </c>
       <c r="C157" t="s">
-        <v>354</v>
+        <v>1047</v>
       </c>
       <c r="D157" t="s">
-        <v>467</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="158" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B158" t="s">
-        <v>456</v>
+        <v>1034</v>
       </c>
       <c r="C158" t="s">
-        <v>228</v>
+        <v>1049</v>
       </c>
       <c r="D158" t="s">
-        <v>128</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="159" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B159" t="s">
-        <v>457</v>
+        <v>1035</v>
       </c>
       <c r="C159" t="s">
-        <v>469</v>
+        <v>1051</v>
       </c>
       <c r="D159" t="s">
-        <v>470</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="160" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B160" t="s">
-        <v>458</v>
+        <v>1036</v>
       </c>
       <c r="C160" t="s">
-        <v>7</v>
+        <v>1053</v>
       </c>
       <c r="D160" t="s">
-        <v>471</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="161" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B161" t="s">
-        <v>459</v>
+        <v>1037</v>
       </c>
       <c r="C161" t="s">
-        <v>472</v>
+        <v>526</v>
       </c>
       <c r="D161" t="s">
-        <v>473</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="162" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B162" t="s">
-        <v>474</v>
+        <v>450</v>
       </c>
       <c r="C162" t="s">
-        <v>485</v>
+        <v>460</v>
       </c>
       <c r="D162" t="s">
-        <v>484</v>
+        <v>461</v>
       </c>
     </row>
     <row r="163" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B163" t="s">
-        <v>475</v>
+        <v>451</v>
       </c>
       <c r="C163" t="s">
-        <v>19</v>
+        <v>462</v>
       </c>
       <c r="D163" t="s">
-        <v>486</v>
+        <v>12</v>
       </c>
     </row>
     <row r="164" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B164" t="s">
-        <v>476</v>
+        <v>452</v>
       </c>
       <c r="C164" t="s">
-        <v>487</v>
+        <v>463</v>
       </c>
       <c r="D164" t="s">
-        <v>11</v>
+        <v>464</v>
       </c>
     </row>
     <row r="165" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B165" t="s">
-        <v>477</v>
+        <v>453</v>
       </c>
       <c r="C165" t="s">
-        <v>27</v>
+        <v>465</v>
       </c>
       <c r="D165" t="s">
-        <v>488</v>
+        <v>466</v>
       </c>
     </row>
     <row r="166" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B166" t="s">
-        <v>478</v>
+        <v>454</v>
       </c>
       <c r="C166" t="s">
-        <v>489</v>
+        <v>17</v>
       </c>
       <c r="D166" t="s">
-        <v>490</v>
+        <v>468</v>
       </c>
     </row>
     <row r="167" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B167" t="s">
-        <v>479</v>
+        <v>455</v>
       </c>
       <c r="C167" t="s">
-        <v>491</v>
+        <v>354</v>
       </c>
       <c r="D167" t="s">
-        <v>492</v>
+        <v>467</v>
       </c>
     </row>
     <row r="168" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B168" t="s">
-        <v>480</v>
+        <v>456</v>
       </c>
       <c r="C168" t="s">
-        <v>493</v>
+        <v>228</v>
       </c>
       <c r="D168" t="s">
-        <v>494</v>
+        <v>128</v>
       </c>
     </row>
     <row r="169" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B169" t="s">
-        <v>481</v>
+        <v>457</v>
       </c>
       <c r="C169" t="s">
-        <v>500</v>
+        <v>469</v>
       </c>
       <c r="D169" t="s">
-        <v>495</v>
+        <v>470</v>
       </c>
     </row>
     <row r="170" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B170" t="s">
-        <v>482</v>
+        <v>458</v>
       </c>
       <c r="C170" t="s">
-        <v>496</v>
+        <v>7</v>
       </c>
       <c r="D170" t="s">
-        <v>497</v>
+        <v>471</v>
       </c>
     </row>
     <row r="171" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B171" t="s">
-        <v>483</v>
+        <v>459</v>
       </c>
       <c r="C171" t="s">
-        <v>498</v>
+        <v>472</v>
       </c>
       <c r="D171" t="s">
-        <v>499</v>
+        <v>473</v>
       </c>
     </row>
     <row r="172" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B172" t="s">
-        <v>501</v>
+        <v>474</v>
       </c>
       <c r="C172" t="s">
-        <v>511</v>
+        <v>485</v>
       </c>
       <c r="D172" t="s">
-        <v>512</v>
+        <v>484</v>
       </c>
     </row>
     <row r="173" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B173" t="s">
-        <v>502</v>
+        <v>475</v>
       </c>
       <c r="C173" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="D173" t="s">
-        <v>513</v>
+        <v>486</v>
       </c>
     </row>
     <row r="174" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B174" t="s">
-        <v>503</v>
+        <v>476</v>
       </c>
       <c r="C174" t="s">
-        <v>514</v>
+        <v>487</v>
       </c>
       <c r="D174" t="s">
-        <v>515</v>
+        <v>11</v>
       </c>
     </row>
     <row r="175" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B175" t="s">
-        <v>504</v>
+        <v>477</v>
       </c>
       <c r="C175" t="s">
-        <v>516</v>
+        <v>27</v>
       </c>
       <c r="D175" t="s">
-        <v>4</v>
+        <v>488</v>
       </c>
     </row>
     <row r="176" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B176" t="s">
-        <v>505</v>
+        <v>478</v>
       </c>
       <c r="C176" t="s">
-        <v>517</v>
+        <v>489</v>
       </c>
       <c r="D176" t="s">
-        <v>309</v>
+        <v>490</v>
       </c>
     </row>
     <row r="177" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B177" t="s">
-        <v>506</v>
+        <v>479</v>
       </c>
       <c r="C177" t="s">
-        <v>520</v>
+        <v>491</v>
       </c>
       <c r="D177" t="s">
-        <v>521</v>
+        <v>492</v>
       </c>
     </row>
     <row r="178" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B178" t="s">
-        <v>507</v>
+        <v>480</v>
       </c>
       <c r="C178" t="s">
-        <v>518</v>
+        <v>493</v>
       </c>
       <c r="D178" t="s">
-        <v>519</v>
+        <v>494</v>
       </c>
     </row>
     <row r="179" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B179" t="s">
-        <v>508</v>
+        <v>481</v>
       </c>
       <c r="C179" t="s">
-        <v>522</v>
+        <v>500</v>
       </c>
       <c r="D179" t="s">
-        <v>523</v>
+        <v>495</v>
       </c>
     </row>
     <row r="180" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B180" t="s">
-        <v>509</v>
+        <v>482</v>
       </c>
       <c r="C180" t="s">
-        <v>524</v>
+        <v>496</v>
       </c>
       <c r="D180" t="s">
-        <v>525</v>
+        <v>497</v>
       </c>
     </row>
     <row r="181" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B181" t="s">
-        <v>510</v>
+        <v>483</v>
       </c>
       <c r="C181" t="s">
-        <v>526</v>
+        <v>498</v>
       </c>
       <c r="D181" t="s">
-        <v>527</v>
+        <v>499</v>
       </c>
     </row>
     <row r="182" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B182" t="s">
-        <v>528</v>
+        <v>501</v>
       </c>
       <c r="C182" t="s">
-        <v>538</v>
+        <v>511</v>
       </c>
       <c r="D182" t="s">
-        <v>539</v>
+        <v>512</v>
       </c>
     </row>
     <row r="183" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B183" t="s">
-        <v>529</v>
+        <v>502</v>
       </c>
       <c r="C183" t="s">
-        <v>161</v>
+        <v>32</v>
       </c>
       <c r="D183" t="s">
-        <v>540</v>
+        <v>513</v>
       </c>
     </row>
     <row r="184" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B184" t="s">
-        <v>530</v>
+        <v>503</v>
       </c>
       <c r="C184" t="s">
-        <v>541</v>
+        <v>514</v>
       </c>
       <c r="D184" t="s">
-        <v>542</v>
+        <v>515</v>
       </c>
     </row>
     <row r="185" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B185" t="s">
-        <v>531</v>
+        <v>504</v>
       </c>
       <c r="C185" t="s">
-        <v>543</v>
+        <v>516</v>
       </c>
       <c r="D185" t="s">
-        <v>544</v>
+        <v>4</v>
       </c>
     </row>
     <row r="186" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B186" t="s">
-        <v>535</v>
+        <v>505</v>
       </c>
       <c r="C186" t="s">
-        <v>548</v>
+        <v>517</v>
       </c>
       <c r="D186" t="s">
-        <v>549</v>
+        <v>309</v>
       </c>
     </row>
     <row r="187" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B187" t="s">
-        <v>532</v>
+        <v>506</v>
       </c>
       <c r="C187" t="s">
-        <v>142</v>
+        <v>520</v>
       </c>
       <c r="D187" t="s">
-        <v>494</v>
+        <v>521</v>
       </c>
     </row>
     <row r="188" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B188" t="s">
-        <v>533</v>
+        <v>507</v>
       </c>
       <c r="C188" t="s">
-        <v>545</v>
+        <v>518</v>
       </c>
       <c r="D188" t="s">
-        <v>335</v>
+        <v>519</v>
       </c>
     </row>
     <row r="189" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B189" t="s">
-        <v>534</v>
+        <v>508</v>
       </c>
       <c r="C189" t="s">
-        <v>546</v>
+        <v>522</v>
       </c>
       <c r="D189" t="s">
-        <v>547</v>
+        <v>523</v>
       </c>
     </row>
     <row r="190" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B190" t="s">
-        <v>536</v>
+        <v>509</v>
       </c>
       <c r="C190" t="s">
-        <v>23</v>
+        <v>524</v>
       </c>
       <c r="D190" t="s">
-        <v>13</v>
+        <v>525</v>
       </c>
     </row>
     <row r="191" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B191" t="s">
-        <v>537</v>
+        <v>510</v>
       </c>
       <c r="C191" t="s">
-        <v>498</v>
+        <v>526</v>
       </c>
       <c r="D191" t="s">
-        <v>550</v>
+        <v>527</v>
       </c>
     </row>
     <row r="192" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B192" t="s">
-        <v>552</v>
+        <v>528</v>
       </c>
       <c r="C192" t="s">
-        <v>553</v>
+        <v>538</v>
       </c>
       <c r="D192" t="s">
-        <v>662</v>
+        <v>539</v>
       </c>
     </row>
     <row r="193" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B193" t="s">
-        <v>554</v>
+        <v>529</v>
       </c>
       <c r="C193" t="s">
-        <v>555</v>
+        <v>161</v>
       </c>
       <c r="D193" t="s">
-        <v>556</v>
+        <v>540</v>
       </c>
     </row>
     <row r="194" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B194" t="s">
-        <v>557</v>
+        <v>530</v>
       </c>
       <c r="C194" t="s">
-        <v>558</v>
+        <v>541</v>
       </c>
       <c r="D194" t="s">
-        <v>559</v>
+        <v>542</v>
       </c>
     </row>
     <row r="195" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B195" t="s">
-        <v>560</v>
+        <v>531</v>
       </c>
       <c r="C195" t="s">
-        <v>561</v>
+        <v>543</v>
       </c>
       <c r="D195" t="s">
-        <v>562</v>
+        <v>544</v>
       </c>
     </row>
     <row r="196" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B196" t="s">
-        <v>563</v>
+        <v>535</v>
       </c>
       <c r="C196" t="s">
-        <v>564</v>
+        <v>548</v>
       </c>
       <c r="D196" t="s">
-        <v>565</v>
+        <v>549</v>
       </c>
     </row>
     <row r="197" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B197" t="s">
-        <v>566</v>
+        <v>532</v>
       </c>
       <c r="C197" t="s">
-        <v>30</v>
+        <v>142</v>
       </c>
       <c r="D197" t="s">
-        <v>567</v>
+        <v>494</v>
       </c>
     </row>
     <row r="198" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B198" t="s">
-        <v>568</v>
+        <v>533</v>
       </c>
       <c r="C198" t="s">
-        <v>569</v>
+        <v>545</v>
       </c>
       <c r="D198" t="s">
-        <v>570</v>
+        <v>335</v>
       </c>
     </row>
     <row r="199" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B199" t="s">
-        <v>571</v>
+        <v>534</v>
       </c>
       <c r="C199" t="s">
-        <v>574</v>
+        <v>546</v>
       </c>
       <c r="D199" t="s">
-        <v>575</v>
+        <v>547</v>
       </c>
     </row>
     <row r="200" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B200" t="s">
-        <v>572</v>
+        <v>536</v>
       </c>
       <c r="C200" t="s">
-        <v>576</v>
+        <v>23</v>
       </c>
       <c r="D200" t="s">
-        <v>577</v>
+        <v>13</v>
       </c>
     </row>
     <row r="201" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B201" t="s">
-        <v>573</v>
+        <v>537</v>
       </c>
       <c r="C201" t="s">
-        <v>578</v>
+        <v>498</v>
       </c>
       <c r="D201" t="s">
-        <v>579</v>
+        <v>550</v>
       </c>
     </row>
     <row r="202" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B202" t="s">
-        <v>580</v>
+        <v>552</v>
       </c>
       <c r="C202" t="s">
-        <v>581</v>
+        <v>553</v>
       </c>
       <c r="D202" t="s">
-        <v>582</v>
+        <v>662</v>
       </c>
     </row>
     <row r="203" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B203" s="4" t="s">
-        <v>583</v>
+      <c r="B203" t="s">
+        <v>554</v>
       </c>
       <c r="C203" t="s">
-        <v>584</v>
+        <v>555</v>
       </c>
       <c r="D203" t="s">
-        <v>567</v>
+        <v>556</v>
       </c>
     </row>
     <row r="204" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B204" t="s">
-        <v>585</v>
+        <v>557</v>
       </c>
       <c r="C204" t="s">
-        <v>586</v>
+        <v>558</v>
       </c>
       <c r="D204" t="s">
-        <v>587</v>
+        <v>559</v>
       </c>
     </row>
     <row r="205" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B205" t="s">
-        <v>588</v>
+        <v>560</v>
       </c>
       <c r="C205" t="s">
-        <v>589</v>
+        <v>561</v>
       </c>
       <c r="D205" t="s">
-        <v>590</v>
+        <v>562</v>
       </c>
     </row>
     <row r="206" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B206" s="4" t="s">
-        <v>591</v>
+      <c r="B206" t="s">
+        <v>563</v>
       </c>
       <c r="C206" t="s">
-        <v>592</v>
+        <v>564</v>
       </c>
       <c r="D206" t="s">
-        <v>593</v>
+        <v>565</v>
       </c>
     </row>
     <row r="207" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B207" t="s">
-        <v>594</v>
+        <v>566</v>
       </c>
       <c r="C207" t="s">
-        <v>595</v>
+        <v>30</v>
       </c>
       <c r="D207" t="s">
-        <v>596</v>
+        <v>567</v>
       </c>
     </row>
     <row r="208" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B208" t="s">
-        <v>597</v>
+        <v>568</v>
       </c>
       <c r="C208" t="s">
-        <v>599</v>
+        <v>569</v>
       </c>
       <c r="D208" t="s">
-        <v>600</v>
+        <v>570</v>
       </c>
     </row>
     <row r="209" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B209" t="s">
-        <v>598</v>
+        <v>571</v>
       </c>
       <c r="C209" t="s">
-        <v>601</v>
+        <v>574</v>
       </c>
       <c r="D209" t="s">
-        <v>602</v>
+        <v>575</v>
       </c>
     </row>
     <row r="210" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B210" t="s">
-        <v>603</v>
+        <v>572</v>
       </c>
       <c r="C210" t="s">
-        <v>605</v>
+        <v>576</v>
       </c>
       <c r="D210" t="s">
-        <v>606</v>
+        <v>577</v>
       </c>
     </row>
     <row r="211" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B211" t="s">
-        <v>604</v>
+        <v>573</v>
       </c>
       <c r="C211" t="s">
-        <v>607</v>
+        <v>578</v>
       </c>
       <c r="D211" t="s">
-        <v>608</v>
+        <v>579</v>
       </c>
     </row>
     <row r="212" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B212" t="s">
-        <v>609</v>
+        <v>580</v>
       </c>
       <c r="C212" t="s">
-        <v>616</v>
+        <v>581</v>
       </c>
       <c r="D212" t="s">
-        <v>617</v>
+        <v>582</v>
       </c>
     </row>
     <row r="213" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B213" t="s">
-        <v>610</v>
+      <c r="B213" s="4" t="s">
+        <v>583</v>
       </c>
       <c r="C213" t="s">
-        <v>618</v>
+        <v>584</v>
       </c>
       <c r="D213" t="s">
-        <v>619</v>
+        <v>567</v>
       </c>
     </row>
     <row r="214" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B214" t="s">
-        <v>611</v>
+        <v>585</v>
       </c>
       <c r="C214" t="s">
-        <v>75</v>
+        <v>586</v>
       </c>
       <c r="D214" t="s">
-        <v>620</v>
+        <v>587</v>
       </c>
     </row>
     <row r="215" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B215" t="s">
-        <v>612</v>
+        <v>588</v>
       </c>
       <c r="C215" t="s">
-        <v>621</v>
+        <v>589</v>
       </c>
       <c r="D215" t="s">
-        <v>622</v>
+        <v>590</v>
       </c>
     </row>
     <row r="216" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B216" t="s">
-        <v>613</v>
+      <c r="B216" s="4" t="s">
+        <v>591</v>
       </c>
       <c r="C216" t="s">
-        <v>623</v>
+        <v>592</v>
       </c>
       <c r="D216" t="s">
-        <v>624</v>
+        <v>593</v>
       </c>
     </row>
     <row r="217" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B217" t="s">
-        <v>614</v>
+        <v>594</v>
       </c>
       <c r="C217" t="s">
-        <v>625</v>
+        <v>595</v>
       </c>
       <c r="D217" t="s">
-        <v>626</v>
+        <v>596</v>
       </c>
     </row>
     <row r="218" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B218" t="s">
-        <v>615</v>
+        <v>597</v>
       </c>
       <c r="C218" t="s">
-        <v>627</v>
+        <v>599</v>
       </c>
       <c r="D218" t="s">
-        <v>628</v>
+        <v>600</v>
       </c>
     </row>
     <row r="219" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B219" t="s">
-        <v>629</v>
+        <v>598</v>
       </c>
       <c r="C219" t="s">
-        <v>393</v>
+        <v>601</v>
       </c>
       <c r="D219" t="s">
-        <v>632</v>
+        <v>602</v>
       </c>
     </row>
     <row r="220" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B220" t="s">
-        <v>630</v>
+        <v>603</v>
       </c>
       <c r="C220" t="s">
-        <v>633</v>
+        <v>605</v>
       </c>
       <c r="D220" t="s">
-        <v>634</v>
+        <v>606</v>
       </c>
     </row>
     <row r="221" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B221" t="s">
-        <v>631</v>
+        <v>604</v>
       </c>
       <c r="C221" t="s">
-        <v>26</v>
+        <v>607</v>
       </c>
       <c r="D221" t="s">
-        <v>635</v>
+        <v>608</v>
       </c>
     </row>
     <row r="222" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B222" t="s">
-        <v>636</v>
+        <v>609</v>
       </c>
       <c r="C222" t="s">
-        <v>643</v>
+        <v>616</v>
       </c>
       <c r="D222" t="s">
-        <v>644</v>
+        <v>617</v>
       </c>
     </row>
     <row r="223" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B223" t="s">
-        <v>637</v>
+        <v>610</v>
       </c>
       <c r="C223" t="s">
-        <v>66</v>
+        <v>618</v>
       </c>
       <c r="D223" t="s">
-        <v>645</v>
+        <v>619</v>
       </c>
     </row>
     <row r="224" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B224" t="s">
-        <v>638</v>
+        <v>611</v>
       </c>
       <c r="C224" t="s">
-        <v>646</v>
+        <v>75</v>
       </c>
       <c r="D224" t="s">
-        <v>237</v>
+        <v>620</v>
       </c>
     </row>
     <row r="225" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B225" t="s">
-        <v>639</v>
+        <v>612</v>
       </c>
       <c r="C225" t="s">
-        <v>647</v>
+        <v>621</v>
       </c>
       <c r="D225" t="s">
-        <v>648</v>
+        <v>622</v>
       </c>
     </row>
     <row r="226" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B226" t="s">
-        <v>640</v>
+        <v>613</v>
       </c>
       <c r="C226" t="s">
-        <v>649</v>
+        <v>623</v>
       </c>
       <c r="D226" t="s">
-        <v>650</v>
+        <v>624</v>
       </c>
     </row>
     <row r="227" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B227" t="s">
-        <v>641</v>
+        <v>614</v>
       </c>
       <c r="C227" t="s">
-        <v>651</v>
+        <v>625</v>
       </c>
       <c r="D227" t="s">
-        <v>652</v>
+        <v>626</v>
       </c>
     </row>
     <row r="228" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B228" t="s">
-        <v>642</v>
+        <v>615</v>
       </c>
       <c r="C228" t="s">
-        <v>165</v>
+        <v>627</v>
       </c>
       <c r="D228" t="s">
-        <v>653</v>
+        <v>628</v>
       </c>
     </row>
     <row r="229" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B229" t="s">
-        <v>654</v>
+        <v>629</v>
       </c>
       <c r="C229" t="s">
-        <v>657</v>
+        <v>393</v>
       </c>
       <c r="D229" t="s">
-        <v>90</v>
+        <v>632</v>
       </c>
     </row>
     <row r="230" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B230" t="s">
-        <v>655</v>
+        <v>630</v>
       </c>
       <c r="C230" t="s">
-        <v>658</v>
+        <v>633</v>
       </c>
       <c r="D230" t="s">
-        <v>659</v>
+        <v>634</v>
       </c>
     </row>
     <row r="231" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B231" t="s">
-        <v>656</v>
+        <v>631</v>
       </c>
       <c r="C231" t="s">
-        <v>660</v>
+        <v>26</v>
       </c>
       <c r="D231" t="s">
-        <v>661</v>
+        <v>635</v>
       </c>
     </row>
     <row r="232" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B232" t="s">
-        <v>663</v>
+        <v>636</v>
       </c>
       <c r="C232" t="s">
-        <v>668</v>
+        <v>643</v>
       </c>
       <c r="D232" t="s">
-        <v>669</v>
+        <v>644</v>
       </c>
     </row>
     <row r="233" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B233" t="s">
-        <v>664</v>
+        <v>637</v>
       </c>
       <c r="C233" t="s">
-        <v>670</v>
+        <v>66</v>
       </c>
       <c r="D233" t="s">
-        <v>671</v>
+        <v>645</v>
       </c>
     </row>
     <row r="234" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B234" t="s">
-        <v>665</v>
+        <v>638</v>
       </c>
       <c r="C234" t="s">
-        <v>672</v>
+        <v>646</v>
       </c>
       <c r="D234" t="s">
-        <v>673</v>
+        <v>237</v>
       </c>
     </row>
     <row r="235" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B235" t="s">
-        <v>666</v>
+        <v>639</v>
       </c>
       <c r="C235" t="s">
-        <v>674</v>
+        <v>647</v>
       </c>
       <c r="D235" t="s">
-        <v>675</v>
+        <v>648</v>
       </c>
     </row>
     <row r="236" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B236" t="s">
-        <v>667</v>
+        <v>640</v>
       </c>
       <c r="C236" t="s">
-        <v>676</v>
+        <v>649</v>
       </c>
       <c r="D236" t="s">
-        <v>677</v>
+        <v>650</v>
       </c>
     </row>
     <row r="237" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B237" t="s">
-        <v>678</v>
+        <v>641</v>
       </c>
       <c r="C237" t="s">
-        <v>683</v>
+        <v>651</v>
       </c>
       <c r="D237" t="s">
-        <v>684</v>
+        <v>652</v>
       </c>
     </row>
     <row r="238" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B238" t="s">
-        <v>679</v>
+        <v>642</v>
       </c>
       <c r="C238" t="s">
-        <v>672</v>
+        <v>165</v>
       </c>
       <c r="D238" t="s">
-        <v>685</v>
+        <v>653</v>
       </c>
     </row>
     <row r="239" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B239" t="s">
-        <v>680</v>
+        <v>654</v>
       </c>
       <c r="C239" t="s">
-        <v>686</v>
+        <v>657</v>
       </c>
       <c r="D239" t="s">
-        <v>687</v>
+        <v>90</v>
       </c>
     </row>
     <row r="240" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B240" t="s">
-        <v>681</v>
+        <v>655</v>
       </c>
       <c r="C240" t="s">
-        <v>688</v>
+        <v>658</v>
       </c>
       <c r="D240" t="s">
-        <v>689</v>
+        <v>659</v>
       </c>
     </row>
     <row r="241" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B241" t="s">
-        <v>682</v>
+        <v>656</v>
       </c>
       <c r="C241" t="s">
-        <v>690</v>
+        <v>660</v>
       </c>
       <c r="D241" t="s">
-        <v>691</v>
+        <v>661</v>
       </c>
     </row>
     <row r="242" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B242" t="s">
-        <v>692</v>
+        <v>663</v>
       </c>
       <c r="C242" t="s">
-        <v>699</v>
+        <v>668</v>
       </c>
       <c r="D242" t="s">
-        <v>700</v>
+        <v>669</v>
       </c>
     </row>
     <row r="243" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B243" t="s">
-        <v>693</v>
+        <v>664</v>
       </c>
       <c r="C243" t="s">
-        <v>701</v>
+        <v>670</v>
       </c>
       <c r="D243" t="s">
-        <v>702</v>
+        <v>671</v>
       </c>
     </row>
     <row r="244" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B244" t="s">
-        <v>694</v>
+        <v>665</v>
       </c>
       <c r="C244" t="s">
-        <v>703</v>
+        <v>672</v>
       </c>
       <c r="D244" t="s">
-        <v>704</v>
+        <v>673</v>
       </c>
     </row>
     <row r="245" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B245" t="s">
-        <v>695</v>
+        <v>666</v>
       </c>
       <c r="C245" t="s">
-        <v>705</v>
+        <v>674</v>
       </c>
       <c r="D245" t="s">
-        <v>706</v>
+        <v>675</v>
       </c>
     </row>
     <row r="246" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B246" t="s">
-        <v>696</v>
+        <v>667</v>
       </c>
       <c r="C246" t="s">
-        <v>707</v>
+        <v>676</v>
       </c>
       <c r="D246" t="s">
-        <v>708</v>
+        <v>677</v>
       </c>
     </row>
     <row r="247" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B247" t="s">
-        <v>697</v>
+        <v>678</v>
       </c>
       <c r="C247" t="s">
-        <v>211</v>
+        <v>683</v>
       </c>
       <c r="D247" t="s">
-        <v>709</v>
+        <v>684</v>
       </c>
     </row>
     <row r="248" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B248" t="s">
-        <v>698</v>
+        <v>679</v>
       </c>
       <c r="C248" t="s">
-        <v>710</v>
+        <v>672</v>
       </c>
       <c r="D248" t="s">
-        <v>711</v>
+        <v>685</v>
       </c>
     </row>
     <row r="249" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B249" t="s">
-        <v>712</v>
+        <v>680</v>
       </c>
       <c r="C249" t="s">
-        <v>715</v>
+        <v>686</v>
       </c>
       <c r="D249" t="s">
-        <v>716</v>
+        <v>687</v>
       </c>
     </row>
     <row r="250" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B250" t="s">
-        <v>713</v>
+        <v>681</v>
       </c>
       <c r="C250" t="s">
-        <v>717</v>
+        <v>688</v>
       </c>
       <c r="D250" t="s">
-        <v>718</v>
+        <v>689</v>
       </c>
     </row>
     <row r="251" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B251" t="s">
-        <v>714</v>
+        <v>682</v>
       </c>
       <c r="C251" t="s">
-        <v>546</v>
+        <v>690</v>
       </c>
       <c r="D251" t="s">
-        <v>719</v>
+        <v>691</v>
       </c>
     </row>
     <row r="252" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B252" t="s">
-        <v>720</v>
+        <v>692</v>
       </c>
       <c r="C252" t="s">
-        <v>725</v>
+        <v>699</v>
       </c>
       <c r="D252" t="s">
-        <v>726</v>
+        <v>700</v>
       </c>
     </row>
     <row r="253" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B253" t="s">
-        <v>721</v>
+        <v>693</v>
       </c>
       <c r="C253" t="s">
-        <v>727</v>
+        <v>701</v>
       </c>
       <c r="D253" t="s">
-        <v>728</v>
+        <v>702</v>
       </c>
     </row>
     <row r="254" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B254" t="s">
-        <v>722</v>
+        <v>694</v>
       </c>
       <c r="C254" t="s">
-        <v>729</v>
+        <v>703</v>
       </c>
       <c r="D254" t="s">
-        <v>730</v>
+        <v>704</v>
       </c>
     </row>
     <row r="255" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B255" s="2" t="s">
-        <v>723</v>
+      <c r="B255" t="s">
+        <v>695</v>
       </c>
       <c r="C255" t="s">
-        <v>731</v>
+        <v>705</v>
       </c>
       <c r="D255" t="s">
-        <v>732</v>
+        <v>706</v>
       </c>
     </row>
     <row r="256" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B256" t="s">
-        <v>733</v>
+        <v>696</v>
       </c>
       <c r="C256" t="s">
-        <v>734</v>
+        <v>707</v>
       </c>
       <c r="D256" t="s">
-        <v>735</v>
+        <v>708</v>
       </c>
     </row>
     <row r="257" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B257" t="s">
-        <v>724</v>
+        <v>697</v>
       </c>
       <c r="C257" t="s">
-        <v>736</v>
+        <v>211</v>
       </c>
       <c r="D257" t="s">
-        <v>737</v>
+        <v>709</v>
       </c>
     </row>
     <row r="258" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B258" t="s">
-        <v>788</v>
+        <v>698</v>
       </c>
       <c r="C258" t="s">
-        <v>514</v>
+        <v>710</v>
       </c>
       <c r="D258" t="s">
-        <v>792</v>
+        <v>711</v>
       </c>
     </row>
     <row r="259" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B259" t="s">
-        <v>789</v>
+        <v>712</v>
       </c>
       <c r="C259" t="s">
-        <v>793</v>
+        <v>715</v>
       </c>
       <c r="D259" t="s">
-        <v>794</v>
+        <v>716</v>
       </c>
     </row>
     <row r="260" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B260" t="s">
-        <v>790</v>
+        <v>713</v>
       </c>
       <c r="C260" t="s">
-        <v>795</v>
+        <v>717</v>
       </c>
       <c r="D260" t="s">
-        <v>796</v>
+        <v>718</v>
       </c>
     </row>
     <row r="261" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B261" t="s">
-        <v>791</v>
+        <v>714</v>
       </c>
       <c r="C261" t="s">
-        <v>757</v>
+        <v>546</v>
       </c>
       <c r="D261" t="s">
-        <v>797</v>
+        <v>719</v>
       </c>
     </row>
     <row r="262" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B262" t="s">
-        <v>738</v>
+        <v>720</v>
       </c>
       <c r="C262" t="s">
-        <v>745</v>
+        <v>725</v>
       </c>
       <c r="D262" t="s">
-        <v>746</v>
+        <v>726</v>
       </c>
     </row>
     <row r="263" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B263" t="s">
-        <v>739</v>
+        <v>721</v>
       </c>
       <c r="C263" t="s">
-        <v>747</v>
+        <v>727</v>
       </c>
       <c r="D263" t="s">
-        <v>748</v>
+        <v>728</v>
       </c>
     </row>
     <row r="264" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B264" t="s">
-        <v>740</v>
+        <v>722</v>
       </c>
       <c r="C264" t="s">
-        <v>749</v>
+        <v>729</v>
       </c>
       <c r="D264" t="s">
-        <v>750</v>
+        <v>730</v>
       </c>
     </row>
     <row r="265" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B265" t="s">
-        <v>741</v>
+      <c r="B265" s="2" t="s">
+        <v>723</v>
       </c>
       <c r="C265" t="s">
-        <v>751</v>
+        <v>731</v>
       </c>
       <c r="D265" t="s">
-        <v>752</v>
+        <v>732</v>
       </c>
     </row>
     <row r="266" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B266" t="s">
-        <v>742</v>
+        <v>733</v>
       </c>
       <c r="C266" t="s">
-        <v>753</v>
+        <v>734</v>
       </c>
       <c r="D266" t="s">
-        <v>754</v>
+        <v>735</v>
       </c>
     </row>
     <row r="267" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B267" t="s">
-        <v>743</v>
+        <v>724</v>
       </c>
       <c r="C267" t="s">
-        <v>755</v>
+        <v>736</v>
       </c>
       <c r="D267" t="s">
-        <v>756</v>
+        <v>737</v>
       </c>
     </row>
     <row r="268" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B268" t="s">
-        <v>744</v>
+        <v>788</v>
       </c>
       <c r="C268" t="s">
-        <v>757</v>
+        <v>514</v>
       </c>
       <c r="D268" t="s">
-        <v>758</v>
+        <v>792</v>
       </c>
     </row>
     <row r="269" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B269" t="s">
-        <v>765</v>
+        <v>789</v>
       </c>
       <c r="C269" t="s">
-        <v>768</v>
+        <v>793</v>
       </c>
       <c r="D269" t="s">
-        <v>381</v>
+        <v>794</v>
       </c>
     </row>
     <row r="270" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B270" t="s">
-        <v>766</v>
+        <v>790</v>
       </c>
       <c r="C270" t="s">
-        <v>769</v>
+        <v>795</v>
       </c>
       <c r="D270" t="s">
-        <v>770</v>
+        <v>796</v>
       </c>
     </row>
     <row r="271" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B271" t="s">
-        <v>767</v>
+        <v>791</v>
       </c>
       <c r="C271" t="s">
-        <v>771</v>
+        <v>757</v>
       </c>
       <c r="D271" t="s">
-        <v>772</v>
+        <v>797</v>
       </c>
     </row>
     <row r="272" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B272" t="s">
-        <v>759</v>
+        <v>738</v>
       </c>
       <c r="C272" t="s">
-        <v>29</v>
+        <v>745</v>
       </c>
       <c r="D272" t="s">
-        <v>773</v>
+        <v>746</v>
       </c>
     </row>
     <row r="273" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B273" t="s">
-        <v>760</v>
+        <v>739</v>
       </c>
       <c r="C273" t="s">
-        <v>727</v>
+        <v>747</v>
       </c>
       <c r="D273" t="s">
-        <v>774</v>
+        <v>748</v>
       </c>
     </row>
     <row r="274" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B274" t="s">
-        <v>798</v>
+        <v>740</v>
       </c>
       <c r="C274" t="s">
-        <v>799</v>
+        <v>749</v>
       </c>
       <c r="D274" t="s">
-        <v>800</v>
+        <v>750</v>
       </c>
     </row>
     <row r="275" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B275" t="s">
-        <v>761</v>
+        <v>741</v>
       </c>
       <c r="C275" t="s">
-        <v>771</v>
+        <v>751</v>
       </c>
       <c r="D275" t="s">
-        <v>64</v>
+        <v>752</v>
       </c>
     </row>
     <row r="276" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B276" t="s">
-        <v>762</v>
+        <v>742</v>
       </c>
       <c r="C276" t="s">
-        <v>775</v>
+        <v>753</v>
       </c>
       <c r="D276" t="s">
-        <v>776</v>
+        <v>754</v>
       </c>
     </row>
     <row r="277" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B277" t="s">
-        <v>763</v>
+        <v>743</v>
       </c>
       <c r="C277" t="s">
-        <v>33</v>
+        <v>755</v>
       </c>
       <c r="D277" t="s">
-        <v>418</v>
+        <v>756</v>
       </c>
     </row>
     <row r="278" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B278" t="s">
-        <v>764</v>
+        <v>744</v>
       </c>
       <c r="C278" t="s">
-        <v>777</v>
+        <v>757</v>
       </c>
       <c r="D278" t="s">
-        <v>778</v>
+        <v>758</v>
       </c>
     </row>
     <row r="279" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B279" t="s">
-        <v>779</v>
+        <v>765</v>
       </c>
       <c r="C279" t="s">
-        <v>782</v>
+        <v>768</v>
       </c>
       <c r="D279" t="s">
-        <v>783</v>
+        <v>381</v>
       </c>
     </row>
     <row r="280" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B280" t="s">
-        <v>780</v>
+        <v>766</v>
       </c>
       <c r="C280" t="s">
-        <v>784</v>
+        <v>769</v>
       </c>
       <c r="D280" t="s">
-        <v>785</v>
+        <v>770</v>
       </c>
     </row>
     <row r="281" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B281" t="s">
-        <v>781</v>
+        <v>767</v>
       </c>
       <c r="C281" t="s">
-        <v>786</v>
+        <v>771</v>
       </c>
       <c r="D281" t="s">
-        <v>787</v>
+        <v>772</v>
       </c>
     </row>
     <row r="282" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B282" t="s">
-        <v>801</v>
+        <v>759</v>
       </c>
       <c r="C282" t="s">
-        <v>810</v>
+        <v>29</v>
       </c>
       <c r="D282" t="s">
-        <v>811</v>
+        <v>773</v>
       </c>
     </row>
     <row r="283" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B283" t="s">
-        <v>802</v>
+        <v>760</v>
       </c>
       <c r="C283" t="s">
-        <v>812</v>
+        <v>727</v>
       </c>
       <c r="D283" t="s">
-        <v>813</v>
+        <v>774</v>
       </c>
     </row>
     <row r="284" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B284" t="s">
-        <v>803</v>
+        <v>798</v>
       </c>
       <c r="C284" t="s">
-        <v>814</v>
+        <v>799</v>
       </c>
       <c r="D284" t="s">
-        <v>825</v>
+        <v>800</v>
       </c>
     </row>
     <row r="285" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B285" t="s">
-        <v>804</v>
+        <v>761</v>
       </c>
       <c r="C285" t="s">
-        <v>54</v>
+        <v>771</v>
       </c>
       <c r="D285" t="s">
-        <v>815</v>
+        <v>64</v>
       </c>
     </row>
     <row r="286" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B286" t="s">
-        <v>805</v>
+        <v>762</v>
       </c>
       <c r="C286" t="s">
-        <v>816</v>
+        <v>775</v>
       </c>
       <c r="D286" t="s">
-        <v>817</v>
+        <v>776</v>
       </c>
     </row>
     <row r="287" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B287" t="s">
-        <v>806</v>
+        <v>763</v>
       </c>
       <c r="C287" t="s">
-        <v>818</v>
+        <v>33</v>
       </c>
       <c r="D287" t="s">
-        <v>819</v>
+        <v>418</v>
       </c>
     </row>
     <row r="288" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B288" t="s">
-        <v>826</v>
+        <v>764</v>
       </c>
       <c r="C288" t="s">
-        <v>827</v>
+        <v>777</v>
       </c>
       <c r="D288" t="s">
-        <v>828</v>
+        <v>778</v>
       </c>
     </row>
     <row r="289" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B289" t="s">
-        <v>807</v>
+        <v>779</v>
       </c>
       <c r="C289" t="s">
-        <v>820</v>
+        <v>782</v>
       </c>
       <c r="D289" t="s">
-        <v>821</v>
+        <v>783</v>
       </c>
     </row>
     <row r="290" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B290" t="s">
-        <v>808</v>
+        <v>780</v>
       </c>
       <c r="C290" t="s">
-        <v>822</v>
+        <v>784</v>
       </c>
       <c r="D290" t="s">
-        <v>484</v>
+        <v>785</v>
       </c>
     </row>
     <row r="291" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B291" t="s">
-        <v>809</v>
+        <v>781</v>
       </c>
       <c r="C291" t="s">
-        <v>823</v>
+        <v>786</v>
       </c>
       <c r="D291" t="s">
-        <v>824</v>
+        <v>787</v>
       </c>
     </row>
     <row r="292" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B292" t="s">
-        <v>829</v>
+        <v>801</v>
       </c>
       <c r="C292" t="s">
-        <v>839</v>
+        <v>810</v>
       </c>
       <c r="D292" t="s">
-        <v>840</v>
+        <v>811</v>
       </c>
     </row>
     <row r="293" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B293" t="s">
-        <v>830</v>
+        <v>802</v>
       </c>
       <c r="C293" t="s">
-        <v>40</v>
+        <v>812</v>
       </c>
       <c r="D293" t="s">
-        <v>841</v>
+        <v>813</v>
       </c>
     </row>
     <row r="294" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B294" t="s">
-        <v>831</v>
+        <v>803</v>
       </c>
       <c r="C294" t="s">
-        <v>842</v>
+        <v>814</v>
       </c>
       <c r="D294" t="s">
-        <v>843</v>
+        <v>825</v>
       </c>
     </row>
     <row r="295" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B295" t="s">
-        <v>832</v>
+        <v>804</v>
       </c>
       <c r="C295" t="s">
-        <v>844</v>
+        <v>54</v>
       </c>
       <c r="D295" t="s">
-        <v>845</v>
+        <v>815</v>
       </c>
     </row>
     <row r="296" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B296" t="s">
-        <v>833</v>
+        <v>805</v>
       </c>
       <c r="C296" t="s">
-        <v>846</v>
+        <v>816</v>
       </c>
       <c r="D296" t="s">
-        <v>847</v>
+        <v>817</v>
       </c>
     </row>
     <row r="297" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B297" t="s">
-        <v>834</v>
+        <v>806</v>
       </c>
       <c r="C297" t="s">
-        <v>848</v>
+        <v>818</v>
       </c>
       <c r="D297" t="s">
-        <v>122</v>
+        <v>819</v>
       </c>
     </row>
     <row r="298" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B298" t="s">
-        <v>835</v>
+        <v>826</v>
       </c>
       <c r="C298" t="s">
-        <v>849</v>
+        <v>827</v>
       </c>
       <c r="D298" t="s">
-        <v>850</v>
+        <v>828</v>
       </c>
     </row>
     <row r="299" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B299" t="s">
-        <v>836</v>
+        <v>807</v>
       </c>
       <c r="C299" t="s">
-        <v>851</v>
+        <v>820</v>
       </c>
       <c r="D299" t="s">
-        <v>852</v>
+        <v>821</v>
       </c>
     </row>
     <row r="300" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B300" t="s">
-        <v>837</v>
+        <v>808</v>
       </c>
       <c r="C300" t="s">
-        <v>853</v>
+        <v>822</v>
       </c>
       <c r="D300" t="s">
-        <v>854</v>
+        <v>484</v>
       </c>
     </row>
     <row r="301" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B301" t="s">
-        <v>838</v>
+        <v>809</v>
       </c>
       <c r="C301" t="s">
-        <v>849</v>
+        <v>823</v>
       </c>
       <c r="D301" t="s">
-        <v>855</v>
+        <v>824</v>
       </c>
     </row>
     <row r="302" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B302" t="s">
-        <v>856</v>
+        <v>829</v>
       </c>
       <c r="C302" t="s">
-        <v>860</v>
+        <v>839</v>
       </c>
       <c r="D302" t="s">
-        <v>861</v>
+        <v>840</v>
       </c>
     </row>
     <row r="303" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B303" t="s">
-        <v>857</v>
+        <v>830</v>
       </c>
       <c r="C303" t="s">
-        <v>862</v>
+        <v>40</v>
       </c>
       <c r="D303" t="s">
-        <v>863</v>
+        <v>841</v>
       </c>
     </row>
     <row r="304" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B304" t="s">
-        <v>858</v>
+        <v>831</v>
       </c>
       <c r="C304" t="s">
-        <v>15</v>
+        <v>842</v>
       </c>
       <c r="D304" t="s">
-        <v>864</v>
+        <v>843</v>
       </c>
     </row>
     <row r="305" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B305" t="s">
-        <v>859</v>
+        <v>832</v>
       </c>
       <c r="C305" t="s">
-        <v>865</v>
+        <v>844</v>
       </c>
       <c r="D305" t="s">
-        <v>866</v>
+        <v>845</v>
       </c>
     </row>
     <row r="306" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B306" t="s">
-        <v>867</v>
+        <v>833</v>
       </c>
       <c r="C306" t="s">
-        <v>873</v>
+        <v>846</v>
       </c>
       <c r="D306" t="s">
-        <v>874</v>
+        <v>847</v>
       </c>
     </row>
     <row r="307" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B307" t="s">
-        <v>868</v>
+        <v>834</v>
       </c>
       <c r="C307" t="s">
-        <v>875</v>
+        <v>848</v>
       </c>
       <c r="D307" t="s">
-        <v>876</v>
+        <v>122</v>
       </c>
     </row>
     <row r="308" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B308" t="s">
-        <v>869</v>
+        <v>835</v>
       </c>
       <c r="C308" t="s">
-        <v>877</v>
+        <v>849</v>
       </c>
       <c r="D308" t="s">
-        <v>878</v>
+        <v>850</v>
       </c>
     </row>
     <row r="309" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B309" t="s">
-        <v>870</v>
+        <v>836</v>
       </c>
       <c r="C309" t="s">
-        <v>879</v>
+        <v>851</v>
       </c>
       <c r="D309" t="s">
-        <v>880</v>
+        <v>852</v>
       </c>
     </row>
     <row r="310" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B310" t="s">
-        <v>871</v>
+        <v>837</v>
       </c>
       <c r="C310" t="s">
-        <v>881</v>
+        <v>853</v>
       </c>
       <c r="D310" t="s">
-        <v>882</v>
+        <v>854</v>
       </c>
     </row>
     <row r="311" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B311" s="2" t="s">
-        <v>872</v>
+      <c r="B311" t="s">
+        <v>838</v>
       </c>
       <c r="C311" t="s">
-        <v>883</v>
+        <v>849</v>
       </c>
       <c r="D311" t="s">
-        <v>884</v>
+        <v>855</v>
       </c>
     </row>
     <row r="312" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B312" t="s">
-        <v>885</v>
+        <v>856</v>
       </c>
       <c r="C312" t="s">
-        <v>895</v>
+        <v>860</v>
       </c>
       <c r="D312" t="s">
-        <v>896</v>
+        <v>861</v>
       </c>
     </row>
     <row r="313" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B313" t="s">
-        <v>886</v>
+        <v>857</v>
       </c>
       <c r="C313" t="s">
-        <v>897</v>
+        <v>862</v>
       </c>
       <c r="D313" t="s">
-        <v>898</v>
+        <v>863</v>
       </c>
     </row>
     <row r="314" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B314" t="s">
-        <v>887</v>
+        <v>858</v>
       </c>
       <c r="C314" t="s">
-        <v>899</v>
+        <v>15</v>
       </c>
       <c r="D314" t="s">
-        <v>912</v>
+        <v>864</v>
       </c>
     </row>
     <row r="315" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B315" t="s">
-        <v>888</v>
+        <v>859</v>
       </c>
       <c r="C315" t="s">
-        <v>524</v>
+        <v>865</v>
       </c>
       <c r="D315" t="s">
-        <v>900</v>
+        <v>866</v>
       </c>
     </row>
     <row r="316" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B316" t="s">
-        <v>889</v>
+        <v>867</v>
       </c>
       <c r="C316" t="s">
-        <v>901</v>
+        <v>873</v>
       </c>
       <c r="D316" t="s">
-        <v>902</v>
+        <v>874</v>
       </c>
     </row>
     <row r="317" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B317" t="s">
-        <v>890</v>
+        <v>868</v>
       </c>
       <c r="C317" t="s">
-        <v>903</v>
+        <v>875</v>
       </c>
       <c r="D317" t="s">
-        <v>904</v>
+        <v>876</v>
       </c>
     </row>
     <row r="318" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B318" t="s">
-        <v>891</v>
+        <v>869</v>
       </c>
       <c r="C318" t="s">
-        <v>905</v>
+        <v>877</v>
       </c>
       <c r="D318" t="s">
-        <v>906</v>
+        <v>878</v>
       </c>
     </row>
     <row r="319" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B319" t="s">
-        <v>892</v>
+        <v>870</v>
       </c>
       <c r="C319" t="s">
-        <v>907</v>
+        <v>879</v>
       </c>
       <c r="D319" t="s">
-        <v>908</v>
+        <v>880</v>
       </c>
     </row>
     <row r="320" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B320" t="s">
-        <v>893</v>
+        <v>871</v>
       </c>
       <c r="C320" t="s">
-        <v>633</v>
+        <v>881</v>
       </c>
       <c r="D320" t="s">
-        <v>909</v>
+        <v>882</v>
       </c>
     </row>
     <row r="321" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B321" t="s">
-        <v>894</v>
+      <c r="B321" s="2" t="s">
+        <v>872</v>
       </c>
       <c r="C321" t="s">
-        <v>910</v>
+        <v>883</v>
       </c>
       <c r="D321" t="s">
-        <v>911</v>
+        <v>884</v>
       </c>
     </row>
     <row r="322" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B322" t="s">
-        <v>913</v>
+        <v>885</v>
       </c>
       <c r="C322" t="s">
-        <v>933</v>
+        <v>895</v>
       </c>
       <c r="D322" t="s">
-        <v>934</v>
+        <v>896</v>
       </c>
     </row>
     <row r="323" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B323" t="s">
-        <v>914</v>
+        <v>886</v>
       </c>
       <c r="C323" t="s">
-        <v>935</v>
+        <v>897</v>
       </c>
       <c r="D323" t="s">
-        <v>936</v>
+        <v>898</v>
       </c>
     </row>
     <row r="324" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B324" s="2" t="s">
-        <v>915</v>
+      <c r="B324" t="s">
+        <v>887</v>
       </c>
       <c r="C324" t="s">
-        <v>937</v>
+        <v>899</v>
       </c>
       <c r="D324" t="s">
-        <v>938</v>
+        <v>912</v>
       </c>
     </row>
     <row r="325" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B325" t="s">
-        <v>916</v>
+        <v>888</v>
       </c>
       <c r="C325" t="s">
-        <v>939</v>
+        <v>524</v>
       </c>
       <c r="D325" t="s">
-        <v>940</v>
+        <v>900</v>
       </c>
     </row>
     <row r="326" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B326" t="s">
-        <v>921</v>
+        <v>889</v>
       </c>
       <c r="C326" t="s">
-        <v>941</v>
+        <v>901</v>
       </c>
       <c r="D326" t="s">
-        <v>942</v>
+        <v>902</v>
       </c>
     </row>
     <row r="327" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B327" t="s">
-        <v>922</v>
+        <v>890</v>
       </c>
       <c r="C327" t="s">
-        <v>943</v>
+        <v>903</v>
       </c>
       <c r="D327" t="s">
-        <v>943</v>
+        <v>904</v>
       </c>
     </row>
     <row r="328" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B328" t="s">
-        <v>923</v>
+        <v>891</v>
       </c>
       <c r="C328" t="s">
-        <v>963</v>
+        <v>905</v>
       </c>
       <c r="D328" t="s">
-        <v>964</v>
+        <v>906</v>
       </c>
     </row>
     <row r="329" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B329" t="s">
-        <v>924</v>
+        <v>892</v>
       </c>
       <c r="C329" t="s">
-        <v>965</v>
+        <v>907</v>
       </c>
       <c r="D329" t="s">
-        <v>966</v>
+        <v>908</v>
       </c>
     </row>
     <row r="330" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B330" t="s">
-        <v>926</v>
+        <v>893</v>
       </c>
       <c r="C330" t="s">
-        <v>967</v>
+        <v>633</v>
       </c>
       <c r="D330" t="s">
-        <v>968</v>
+        <v>909</v>
       </c>
     </row>
     <row r="331" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B331" t="s">
-        <v>927</v>
+        <v>894</v>
       </c>
       <c r="C331" t="s">
-        <v>969</v>
+        <v>910</v>
       </c>
       <c r="D331" t="s">
-        <v>970</v>
+        <v>911</v>
       </c>
     </row>
     <row r="332" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B332" t="s">
-        <v>928</v>
+        <v>913</v>
       </c>
       <c r="C332" t="s">
-        <v>971</v>
+        <v>933</v>
       </c>
       <c r="D332" t="s">
-        <v>972</v>
+        <v>934</v>
       </c>
     </row>
     <row r="333" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B333" t="s">
-        <v>929</v>
+        <v>914</v>
       </c>
       <c r="C333" t="s">
-        <v>973</v>
+        <v>935</v>
       </c>
       <c r="D333" t="s">
-        <v>974</v>
+        <v>936</v>
       </c>
     </row>
     <row r="334" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B334" t="s">
-        <v>917</v>
+      <c r="B334" s="2" t="s">
+        <v>915</v>
       </c>
       <c r="C334" t="s">
-        <v>975</v>
+        <v>937</v>
       </c>
       <c r="D334" t="s">
-        <v>976</v>
+        <v>938</v>
       </c>
     </row>
     <row r="335" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B335" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="C335" t="s">
-        <v>977</v>
+        <v>939</v>
       </c>
       <c r="D335" t="s">
-        <v>978</v>
+        <v>940</v>
       </c>
     </row>
     <row r="336" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B336" t="s">
-        <v>919</v>
+        <v>921</v>
       </c>
       <c r="C336" t="s">
-        <v>979</v>
+        <v>941</v>
       </c>
       <c r="D336" t="s">
-        <v>980</v>
+        <v>942</v>
       </c>
     </row>
     <row r="337" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B337" t="s">
-        <v>920</v>
+        <v>922</v>
       </c>
       <c r="C337" t="s">
-        <v>981</v>
+        <v>943</v>
       </c>
       <c r="D337" t="s">
-        <v>982</v>
+        <v>943</v>
       </c>
     </row>
     <row r="338" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B338" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
       <c r="C338" t="s">
-        <v>20</v>
+        <v>963</v>
       </c>
       <c r="D338" t="s">
-        <v>968</v>
+        <v>964</v>
       </c>
     </row>
     <row r="339" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B339" t="s">
-        <v>930</v>
+        <v>924</v>
       </c>
       <c r="C339" t="s">
-        <v>983</v>
+        <v>965</v>
       </c>
       <c r="D339" t="s">
-        <v>984</v>
+        <v>966</v>
       </c>
     </row>
     <row r="340" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B340" t="s">
-        <v>1026</v>
+        <v>926</v>
       </c>
       <c r="C340" t="s">
-        <v>782</v>
+        <v>967</v>
       </c>
       <c r="D340" t="s">
-        <v>1027</v>
+        <v>968</v>
       </c>
     </row>
     <row r="341" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B341" t="s">
-        <v>931</v>
+        <v>927</v>
       </c>
       <c r="C341" t="s">
-        <v>985</v>
+        <v>969</v>
       </c>
       <c r="D341" t="s">
-        <v>986</v>
+        <v>970</v>
       </c>
     </row>
     <row r="342" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B342" t="s">
-        <v>932</v>
+        <v>928</v>
       </c>
       <c r="C342" t="s">
-        <v>987</v>
+        <v>971</v>
       </c>
       <c r="D342" t="s">
-        <v>988</v>
+        <v>972</v>
       </c>
     </row>
     <row r="343" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B343" t="s">
-        <v>944</v>
+        <v>929</v>
       </c>
       <c r="C343" t="s">
-        <v>989</v>
+        <v>973</v>
       </c>
       <c r="D343" t="s">
-        <v>70</v>
+        <v>974</v>
       </c>
     </row>
     <row r="344" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B344" t="s">
-        <v>945</v>
+        <v>917</v>
       </c>
       <c r="C344" t="s">
-        <v>990</v>
+        <v>975</v>
       </c>
       <c r="D344" t="s">
-        <v>991</v>
+        <v>976</v>
       </c>
     </row>
     <row r="345" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B345" t="s">
-        <v>946</v>
+        <v>918</v>
       </c>
       <c r="C345" t="s">
-        <v>992</v>
+        <v>977</v>
       </c>
       <c r="D345" t="s">
-        <v>993</v>
+        <v>978</v>
       </c>
     </row>
     <row r="346" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B346" t="s">
-        <v>947</v>
+        <v>919</v>
       </c>
       <c r="C346" t="s">
-        <v>994</v>
+        <v>979</v>
       </c>
       <c r="D346" t="s">
-        <v>995</v>
+        <v>980</v>
       </c>
     </row>
     <row r="347" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B347" t="s">
-        <v>948</v>
+        <v>920</v>
       </c>
       <c r="C347" t="s">
-        <v>996</v>
+        <v>981</v>
       </c>
       <c r="D347" t="s">
-        <v>997</v>
+        <v>982</v>
       </c>
     </row>
     <row r="348" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B348" t="s">
-        <v>949</v>
+        <v>925</v>
       </c>
       <c r="C348" t="s">
-        <v>998</v>
+        <v>20</v>
       </c>
       <c r="D348" t="s">
-        <v>999</v>
+        <v>968</v>
       </c>
     </row>
     <row r="349" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B349" t="s">
-        <v>950</v>
+        <v>930</v>
       </c>
       <c r="C349" t="s">
-        <v>1000</v>
+        <v>983</v>
       </c>
       <c r="D349" t="s">
-        <v>1001</v>
+        <v>984</v>
       </c>
     </row>
     <row r="350" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B350" t="s">
-        <v>951</v>
+        <v>1026</v>
       </c>
       <c r="C350" t="s">
-        <v>1002</v>
+        <v>782</v>
       </c>
       <c r="D350" t="s">
-        <v>1003</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="351" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B351" t="s">
-        <v>952</v>
+        <v>931</v>
       </c>
       <c r="C351" t="s">
-        <v>1004</v>
+        <v>985</v>
       </c>
       <c r="D351" t="s">
-        <v>1005</v>
+        <v>986</v>
       </c>
     </row>
     <row r="352" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B352" t="s">
-        <v>953</v>
+        <v>932</v>
       </c>
       <c r="C352" t="s">
-        <v>1006</v>
+        <v>987</v>
       </c>
       <c r="D352" t="s">
-        <v>1007</v>
+        <v>988</v>
       </c>
     </row>
     <row r="353" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B353" t="s">
-        <v>954</v>
+        <v>944</v>
       </c>
       <c r="C353" t="s">
-        <v>1008</v>
+        <v>989</v>
       </c>
       <c r="D353" t="s">
-        <v>737</v>
+        <v>70</v>
       </c>
     </row>
     <row r="354" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B354" t="s">
-        <v>955</v>
+        <v>945</v>
       </c>
       <c r="C354" t="s">
-        <v>15</v>
+        <v>990</v>
       </c>
       <c r="D354" t="s">
-        <v>1009</v>
+        <v>991</v>
       </c>
     </row>
     <row r="355" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B355" t="s">
-        <v>956</v>
+        <v>946</v>
       </c>
       <c r="C355" t="s">
-        <v>1010</v>
+        <v>992</v>
       </c>
       <c r="D355" t="s">
-        <v>1011</v>
+        <v>993</v>
       </c>
     </row>
     <row r="356" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B356" t="s">
-        <v>957</v>
+        <v>947</v>
       </c>
       <c r="C356" t="s">
-        <v>1012</v>
+        <v>994</v>
       </c>
       <c r="D356" t="s">
-        <v>1013</v>
+        <v>995</v>
       </c>
     </row>
     <row r="357" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B357" t="s">
-        <v>958</v>
+        <v>948</v>
       </c>
       <c r="C357" t="s">
-        <v>1014</v>
+        <v>996</v>
       </c>
       <c r="D357" t="s">
-        <v>1011</v>
+        <v>997</v>
       </c>
     </row>
     <row r="358" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B358" t="s">
-        <v>959</v>
+        <v>949</v>
       </c>
       <c r="C358" t="s">
-        <v>1015</v>
+        <v>998</v>
       </c>
       <c r="D358" t="s">
-        <v>1016</v>
+        <v>999</v>
       </c>
     </row>
     <row r="359" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B359" t="s">
-        <v>960</v>
+        <v>950</v>
       </c>
       <c r="C359" t="s">
-        <v>1017</v>
+        <v>1000</v>
       </c>
       <c r="D359" t="s">
-        <v>1018</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="360" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B360" t="s">
-        <v>961</v>
+        <v>951</v>
       </c>
       <c r="C360" t="s">
-        <v>1019</v>
+        <v>1002</v>
       </c>
       <c r="D360" t="s">
-        <v>1020</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="361" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B361" t="s">
-        <v>962</v>
+        <v>952</v>
       </c>
       <c r="C361" t="s">
-        <v>1021</v>
+        <v>1004</v>
       </c>
       <c r="D361" t="s">
-        <v>1022</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="362" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B362" t="s">
+        <v>953</v>
+      </c>
+      <c r="C362" t="s">
+        <v>1006</v>
+      </c>
+      <c r="D362" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="363" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B363" t="s">
+        <v>954</v>
+      </c>
+      <c r="C363" t="s">
+        <v>1008</v>
+      </c>
+      <c r="D363" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="364" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B364" t="s">
+        <v>955</v>
+      </c>
+      <c r="C364" t="s">
+        <v>15</v>
+      </c>
+      <c r="D364" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="365" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B365" t="s">
+        <v>956</v>
+      </c>
+      <c r="C365" t="s">
+        <v>1010</v>
+      </c>
+      <c r="D365" t="s">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="366" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B366" t="s">
+        <v>957</v>
+      </c>
+      <c r="C366" t="s">
+        <v>1012</v>
+      </c>
+      <c r="D366" t="s">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="367" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B367" t="s">
+        <v>958</v>
+      </c>
+      <c r="C367" t="s">
+        <v>1014</v>
+      </c>
+      <c r="D367" t="s">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="368" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B368" t="s">
+        <v>959</v>
+      </c>
+      <c r="C368" t="s">
+        <v>1015</v>
+      </c>
+      <c r="D368" t="s">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="369" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B369" t="s">
+        <v>960</v>
+      </c>
+      <c r="C369" t="s">
+        <v>1017</v>
+      </c>
+      <c r="D369" t="s">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="370" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B370" t="s">
+        <v>961</v>
+      </c>
+      <c r="C370" t="s">
+        <v>1019</v>
+      </c>
+      <c r="D370" t="s">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="371" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B371" t="s">
+        <v>962</v>
+      </c>
+      <c r="C371" t="s">
+        <v>1021</v>
+      </c>
+      <c r="D371" t="s">
+        <v>1022</v>
+      </c>
+    </row>
+    <row r="372" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B372" t="s">
         <v>1023</v>
       </c>
-      <c r="C362" t="s">
+      <c r="C372" t="s">
         <v>1024</v>
       </c>
-      <c r="D362" t="s">
+      <c r="D372" t="s">
         <v>1025</v>
       </c>
     </row>
-    <row r="365" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B365" s="2"/>
-    </row>
-    <row r="376" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B376" s="2"/>
+    <row r="375" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B375" s="2"/>
+    </row>
+    <row r="386" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B386" s="2"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B52">
     <cfRule type="duplicateValues" dxfId="1" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B316:B1048576 B293:B311 B280:B291 B1:B278">
+  <conditionalFormatting sqref="B326:B1048576 B303:B321 B290:B301 B1:B288">
     <cfRule type="duplicateValues" dxfId="0" priority="7"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>